<commit_message>
update NOTES.xlsx and submissions/full_densenet121_AutoWtdCE_2020-11-27_0-52_epoch49.csv
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8032C2-6E8B-45BB-84A7-7D688526F752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139023C9-013C-43A0-8D84-05ACD1B3DE51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Submissions</t>
   </si>
@@ -59,13 +59,22 @@
   <si>
     <t>add random brightness to preprocess</t>
   </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>full_densenet121_AutoWtdCE_2020-11-27_0-52_epoch49</t>
+  </si>
+  <si>
+    <t>training from scratch and using training preprocess</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-1010409]d\ mmm\ yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1010409]d\ mmm\ yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -122,17 +131,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -365,17 +374,20 @@
           </c:dLbls>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$48</c:f>
+              <c:f>Sheet1!$D$2:$D$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.41199999999999998</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.42099999999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.14499999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -1170,15 +1182,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>307975</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1208,13 +1220,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:D48" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:D48" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:E49" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:E49" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions"/>
-    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model"/>
+    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score"/>
-    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1483,86 +1496,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>44160</v>
+      </c>
+      <c r="D2">
+        <v>0.15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5">
         <v>44162</v>
       </c>
-      <c r="C2">
+      <c r="D3">
         <v>0.41199999999999998</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
         <v>44166</v>
       </c>
-      <c r="C3">
+      <c r="D4">
         <v>0.42099999999999999</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5">
         <v>44167</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>0.14499999999999999</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="5">
         <v>44168</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
fixed preprocess.py (add rotate) change folder structure change net to densenet201
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139023C9-013C-43A0-8D84-05ACD1B3DE51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2F48F3-AC89-496B-BD49-AAEA0B5D356F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Submissions</t>
   </si>
@@ -57,9 +57,6 @@
     <t>using pretrained weights and using training preprocess</t>
   </si>
   <si>
-    <t>add random brightness to preprocess</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -67,6 +64,30 @@
   </si>
   <si>
     <t>training from scratch and using training preprocess</t>
+  </si>
+  <si>
+    <t>novoting_full_densenet121_AutoWtdCE_2020-12-03_1-12_epoch49</t>
+  </si>
+  <si>
+    <t>full_densenet121_AutoWtdCE_2020-12-03_1-12_epoch49</t>
+  </si>
+  <si>
+    <t>voting_full_densenet121_AutoWtdCE_2020-12-03_1-12_epoch49</t>
+  </si>
+  <si>
+    <t>add random increase brightness to preprocess</t>
+  </si>
+  <si>
+    <t>add random increase brightness to preprocess and using voting</t>
+  </si>
+  <si>
+    <t>full_densenet121_AutoWtdCE_2020-12-03_18-35_epoch49</t>
+  </si>
+  <si>
+    <t>voting_full_densenet121_AutoWtdCE_2020-12-03_18-35_epoch49</t>
+  </si>
+  <si>
+    <t>novoting_full_densenet121_AutoWtdCE_2020-12-03_18-35_epoch48</t>
   </si>
 </sst>
 </file>
@@ -119,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -130,18 +151,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -389,6 +436,18 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.43099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16500000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,14 +1279,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:E49" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:E49" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E49" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions"/>
-    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score"/>
-    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1499,15 +1558,15 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="70.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1516,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -1529,209 +1588,380 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5">
         <v>44160</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>0.15</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>44162</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>0.41199999999999998</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5">
         <v>44166</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>0.42099999999999999</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="5">
         <v>44167</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>0.14499999999999999</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="C6" s="5">
         <v>44168</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
+      <c r="D6" s="4">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5">
+        <v>44168</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
+      <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5">
+        <v>44168</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5">
+        <v>44168</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="5"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="5"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="5"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="5"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="5"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="5"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
       <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
       <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
       <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
       <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
       <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
       <c r="C46" s="5"/>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
       <c r="C47" s="5"/>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
       <c r="C48" s="5"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
       <c r="C49" s="5"/>
+      <c r="E49" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
fix data split scheme change the way to save checkpoints fix weight balance formula additional notes on results and training methods
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2F48F3-AC89-496B-BD49-AAEA0B5D356F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B144D2-E3BE-4008-965B-055D256D1542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="results" sheetId="1" r:id="rId1"/>
+    <sheet name="formula note" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>Submissions</t>
   </si>
@@ -39,12 +40,6 @@
     <t>voting_test_full_densenet121_AutoWtdCE_2020-11-30_18-13_epoch99</t>
   </si>
   <si>
-    <t>using pretrained weights and not doing training preprocess</t>
-  </si>
-  <si>
-    <t>same as above with voting after cropping image into 20 pieces size (300x400)</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -54,18 +49,12 @@
     <t>Note</t>
   </si>
   <si>
-    <t>using pretrained weights and using training preprocess</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
     <t>full_densenet121_AutoWtdCE_2020-11-27_0-52_epoch49</t>
   </si>
   <si>
-    <t>training from scratch and using training preprocess</t>
-  </si>
-  <si>
     <t>novoting_full_densenet121_AutoWtdCE_2020-12-03_1-12_epoch49</t>
   </si>
   <si>
@@ -75,12 +64,6 @@
     <t>voting_full_densenet121_AutoWtdCE_2020-12-03_1-12_epoch49</t>
   </si>
   <si>
-    <t>add random increase brightness to preprocess</t>
-  </si>
-  <si>
-    <t>add random increase brightness to preprocess and using voting</t>
-  </si>
-  <si>
     <t>full_densenet121_AutoWtdCE_2020-12-03_18-35_epoch49</t>
   </si>
   <si>
@@ -88,6 +71,137 @@
   </si>
   <si>
     <t>novoting_full_densenet121_AutoWtdCE_2020-12-03_18-35_epoch48</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>old split scheme</t>
+  </si>
+  <si>
+    <t>novoting_full_densenet201_AutoWtdCE_2020-12-04_0-49_epoch49</t>
+  </si>
+  <si>
+    <t>Voting</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>full_densenet201_AutoWtdCE_2020-12-04_0-49_epoch49</t>
+  </si>
+  <si>
+    <t>DATA NOTE:
+OLD SPLIT SCHEME: GET
+   -  80% FROM BEGINNING DOWN OF THE CSV FILE FOR TRAINING
+   -  20% FROM THE END UP OF THE CSV FILE FOR VALIDATION
+NEW SPLIT SCHEME: 
+   -  FOR EVERY CATEGORY, TAKE 1 IMAGE FOR VALIDATION EVERY 5 IMAGES
+   -  OTHER 5 IMAGES ARE PUT INTO TRAINING LIST</t>
+  </si>
+  <si>
+    <t>new split scheme</t>
+  </si>
+  <si>
+    <t>Batch size</t>
+  </si>
+  <si>
+    <t>full_densenet121_AutoWtdCE_2020-12-05_2-56_epoch26</t>
+  </si>
+  <si>
+    <t>novoting_full_densenet121_AutoWtdCE_2020-12-05_2-56_epoch26</t>
+  </si>
+  <si>
+    <t>training from scratch and using training preprocess (wrong weight calculation)</t>
+  </si>
+  <si>
+    <t>using pretrained weights and using training preprocess for testing  (wrong weight calculation)</t>
+  </si>
+  <si>
+    <t>using pretrained weights and not doing training preprocess for testing  (wrong weight calculation)</t>
+  </si>
+  <si>
+    <t>same as above with voting after cropping image into 20 pieces size (300x400)  (wrong weight calculation)</t>
+  </si>
+  <si>
+    <t>add random increase brightness to preprocess and using voting  (wrong weight calculation)</t>
+  </si>
+  <si>
+    <t>add random increase brightness to preprocess  (wrong weight calculation)</t>
+  </si>
+  <si>
+    <t>change model to densenet 201  (wrong weight calculation)</t>
+  </si>
+  <si>
+    <t>using densenet 121 with new data and weight with best val loss  (wrong weight calculation)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>class imbalanced weighted:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+wj=n_samples / (n_classes * n_samplesj)   [1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Here,
+  - wj is the weight for each class(j signifies the class)
+  - n_samplesis the total number of samples or rows in the dataset
+  - n_classesis the total number of unique classes in the target
+  - n_samplesjis the total number of rows of the respective class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">fix weight calculation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[1]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -97,7 +211,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010409]d\ mmm\ yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +229,28 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -158,34 +294,55 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -243,7 +400,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -256,7 +413,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
               <a:t>'Score'</a:t>
             </a:r>
           </a:p>
@@ -275,7 +432,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -370,13 +527,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -421,7 +576,7 @@
           </c:dLbls>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$49</c:f>
+              <c:f>results!$D$2:$D$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
@@ -448,6 +603,12 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.16500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45200000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -513,7 +674,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -560,7 +721,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -592,7 +753,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -624,7 +785,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -682,7 +843,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1241,16 +1402,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>307975</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>605632</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>24607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>100807</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1279,13 +1440,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:E49" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E49" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:H49" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H49" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{2BE8C86F-4F93-4A52-8C5D-56BB4CB29FE4}" name="Data" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{6E53C4CB-4A70-41F7-B3E6-AC55510650BC}" name="Voting" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{1ABD848E-ABED-4151-A1D7-F38492E6213F}" name="Batch size" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1555,415 +1719,611 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="50.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="9">
         <v>44160</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="8">
         <v>0.15</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+    </row>
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9">
         <v>44162</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="8">
         <v>0.41199999999999998</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="8">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="9">
         <v>44166</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="8">
         <v>0.42099999999999999</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="8">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="9">
         <v>44167</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="8">
         <v>0.14499999999999999</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9">
+        <v>44168</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="8">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9">
+        <v>44168</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="9">
+        <v>44168</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="8">
+        <v>12</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="9">
         <v>44168</v>
       </c>
-      <c r="D6" s="4">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="D9" s="8">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5">
-        <v>44168</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.16</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8">
+        <v>12</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5">
-        <v>44168</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9">
+        <v>44169</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="F10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5">
-        <v>44168</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="8">
+        <v>8</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="9">
+        <v>44170</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="8">
+        <v>12</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="9">
+        <v>44170</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="8">
+        <v>12</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="5"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="5"/>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="5"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="5"/>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="5"/>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="5"/>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="5"/>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="5"/>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="5"/>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="5"/>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="5"/>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="5"/>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="5"/>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="5"/>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="5"/>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="5"/>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="5"/>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="5"/>
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="5"/>
-      <c r="E45" s="7"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="5"/>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="5"/>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="5"/>
-      <c r="E49" s="7"/>
+      <c r="H49" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J2:Q8"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1972,4 +2332,30 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEC87F6-42EF-4C28-A44C-D458D6A8AE94}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1048576"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
now use rotate, brightness in preprocess.py fix distort mapping x and y to actual correct result fix test dataloader in submissions.py to suitable new dataloader print best epoch in train.py
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B144D2-E3BE-4008-965B-055D256D1542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253F8D93-4008-4352-B4F1-E867E11957CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,18 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Submissions</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-11-25_1-18</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-11-30_18-13_epoch99</t>
-  </si>
-  <si>
-    <t>voting_test_full_densenet121_AutoWtdCE_2020-11-30_18-13_epoch99</t>
   </si>
   <si>
     <t>Date</t>
@@ -52,36 +43,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>full_densenet121_AutoWtdCE_2020-11-27_0-52_epoch49</t>
-  </si>
-  <si>
-    <t>novoting_full_densenet121_AutoWtdCE_2020-12-03_1-12_epoch49</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-12-03_1-12_epoch49</t>
-  </si>
-  <si>
-    <t>voting_full_densenet121_AutoWtdCE_2020-12-03_1-12_epoch49</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-12-03_18-35_epoch49</t>
-  </si>
-  <si>
-    <t>voting_full_densenet121_AutoWtdCE_2020-12-03_18-35_epoch49</t>
-  </si>
-  <si>
-    <t>novoting_full_densenet121_AutoWtdCE_2020-12-03_18-35_epoch48</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>old split scheme</t>
-  </si>
-  <si>
-    <t>novoting_full_densenet201_AutoWtdCE_2020-12-04_0-49_epoch49</t>
-  </si>
-  <si>
     <t>Voting</t>
   </si>
   <si>
@@ -91,52 +52,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>full_densenet201_AutoWtdCE_2020-12-04_0-49_epoch49</t>
-  </si>
-  <si>
-    <t>DATA NOTE:
-OLD SPLIT SCHEME: GET
-   -  80% FROM BEGINNING DOWN OF THE CSV FILE FOR TRAINING
-   -  20% FROM THE END UP OF THE CSV FILE FOR VALIDATION
-NEW SPLIT SCHEME: 
-   -  FOR EVERY CATEGORY, TAKE 1 IMAGE FOR VALIDATION EVERY 5 IMAGES
-   -  OTHER 5 IMAGES ARE PUT INTO TRAINING LIST</t>
-  </si>
-  <si>
-    <t>new split scheme</t>
-  </si>
-  <si>
     <t>Batch size</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-12-05_2-56_epoch26</t>
-  </si>
-  <si>
-    <t>novoting_full_densenet121_AutoWtdCE_2020-12-05_2-56_epoch26</t>
-  </si>
-  <si>
-    <t>training from scratch and using training preprocess (wrong weight calculation)</t>
-  </si>
-  <si>
-    <t>using pretrained weights and using training preprocess for testing  (wrong weight calculation)</t>
-  </si>
-  <si>
-    <t>using pretrained weights and not doing training preprocess for testing  (wrong weight calculation)</t>
-  </si>
-  <si>
-    <t>same as above with voting after cropping image into 20 pieces size (300x400)  (wrong weight calculation)</t>
-  </si>
-  <si>
-    <t>add random increase brightness to preprocess and using voting  (wrong weight calculation)</t>
-  </si>
-  <si>
-    <t>add random increase brightness to preprocess  (wrong weight calculation)</t>
-  </si>
-  <si>
-    <t>change model to densenet 201  (wrong weight calculation)</t>
-  </si>
-  <si>
-    <t>using densenet 121 with new data and weight with best val loss  (wrong weight calculation)</t>
   </si>
   <si>
     <r>
@@ -189,19 +105,31 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">fix weight calculation </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[1]</t>
-    </r>
+    <t>novoting_full_densenet121_AutoWtdCE_2020-12-05_13-22_epoch46</t>
+  </si>
+  <si>
+    <t>full_densenet121_AutoWtdCE_2020-12-05_13-22_epoch46</t>
+  </si>
+  <si>
+    <t>Epoch</t>
+  </si>
+  <si>
+    <t>novoting_full_densenet121_AutoWtdCE_2020-12-05_13-22_epoch49</t>
+  </si>
+  <si>
+    <t>full_densenet121_AutoWtdCE_2020-12-05_13-22_epoch49</t>
+  </si>
+  <si>
+    <t>add random brightness, rotate</t>
+  </si>
+  <si>
+    <t>bets val loss</t>
+  </si>
+  <si>
+    <t>last epoch</t>
+  </si>
+  <si>
+    <t>change lr from 0.001 to 0.01</t>
   </si>
 </sst>
 </file>
@@ -305,14 +233,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -320,14 +248,7 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -339,10 +260,17 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -457,9 +385,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Score</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -576,39 +501,18 @@
           </c:dLbls>
           <c:yVal>
             <c:numRef>
-              <c:f>results!$D$2:$D$49</c:f>
+              <c:f>results!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.15</c:v>
+                  <c:v>0.751</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41199999999999998</c:v>
+                  <c:v>0.751</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.14499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.41599999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.43099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.16500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.45500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.45200000000000001</c:v>
+                  <c:v>0.16400000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1402,16 +1306,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>605632</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>24607</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>22226</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>167482</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>214313</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>100807</xdr:rowOff>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>29369</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1440,17 +1344,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:H49" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H49" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:H39" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H39" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{2BE8C86F-4F93-4A52-8C5D-56BB4CB29FE4}" name="Data" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{6E53C4CB-4A70-41F7-B3E6-AC55510650BC}" name="Voting" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{1ABD848E-ABED-4151-A1D7-F38492E6213F}" name="Batch size" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{6E53C4CB-4A70-41F7-B3E6-AC55510650BC}" name="Voting" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{1ABD848E-ABED-4151-A1D7-F38492E6213F}" name="Batch size" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{9E6EDDE2-5951-49F3-BEC8-6D7190A570DA}" name="Epoch" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1719,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,363 +1644,234 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C2" s="9">
-        <v>44160</v>
-      </c>
-      <c r="D2" s="8">
-        <v>0.15</v>
+        <v>44170</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.751</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8">
+        <v>50</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="8">
-        <v>12</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" s="9">
-        <v>44162</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.41199999999999998</v>
+        <v>44170</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.751</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="F3" s="8">
+        <v>12</v>
       </c>
       <c r="G3" s="8">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C4" s="9">
-        <v>44166</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0.42099999999999999</v>
+        <v>44170</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.16400000000000001</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="F4" s="8">
+        <v>12</v>
       </c>
       <c r="G4" s="8">
+        <v>50</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+    </row>
+    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="9">
+        <v>44170</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="8">
         <v>12</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="9">
-        <v>44167</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="G5" s="8">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+    </row>
+    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="9">
-        <v>44168</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0.41599999999999998</v>
+        <v>44170</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="F6" s="8">
+        <v>24</v>
       </c>
       <c r="G6" s="8">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="9">
-        <v>44168</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.16</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="8">
-        <v>12</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-    </row>
-    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="9">
-        <v>44168</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="8">
-        <v>12</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-    </row>
-    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="9">
-        <v>44168</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="8">
-        <v>12</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="9">
-        <v>44169</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="8">
-        <v>8</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="9">
-        <v>44170</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.45200000000000001</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="8">
-        <v>12</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+    </row>
+    <row r="7" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+    </row>
+    <row r="8" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="9">
-        <v>44170</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="8">
-        <v>12</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="C12" s="5"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -2260,70 +2035,7 @@
       <c r="C39" s="5"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5"/>
-      <c r="H42" s="6"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5"/>
-      <c r="H43" s="6"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="5"/>
-      <c r="H44" s="6"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="5"/>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5"/>
-      <c r="H48" s="6"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="5"/>
-      <c r="H49" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="J2:Q8"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2348,8 +2060,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>35</v>
+      <c r="A1" s="10" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update new folder structure update working ArcMarginModel.py working m and scale for ArcMarginModel.py update new results and NOTES.xlsx add FocalLoss.py and cosface_pytorch.py for references
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E2D95B-F72D-44D8-9E8F-3D2B033EBC16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA16A7CC-818B-4D5D-8A74-3F319A84A045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Submissions</t>
   </si>
@@ -76,16 +76,7 @@
     <t>last epoch</t>
   </si>
   <si>
-    <t>change lr from 0.001 to 0.01 (failed, val loss exploded)</t>
-  </si>
-  <si>
     <t>add random brightness, rotate, best val loss</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-12-05_14-59_epoch49</t>
   </si>
   <si>
     <t>add random brightness, rotate, last epoch</t>
@@ -154,6 +145,75 @@
   - n_classesis the total number of unique classes in the target
   - n_samplesjis the total number of rows of the respective class</t>
     </r>
+  </si>
+  <si>
+    <t>novoting_densenet121_ArcMargin_2020-12-27_12-36_epoch141</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-27_12-36_epoch141</t>
+  </si>
+  <si>
+    <t>novoting_densenet121_ArcMargin_2020-12-28_0-41_epoch44</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-28_0-41_epoch44</t>
+  </si>
+  <si>
+    <t>arccos margin, s=5, m=0.05, lr=0.01, decay epoch=[43]</t>
+  </si>
+  <si>
+    <t>novoting_densenet121_ArcMargin_2020-12-28_0-36_epoch55</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-28_0-36_epoch55</t>
+  </si>
+  <si>
+    <t>arccos margin, s=5, m=0.1, lr=0.01, decay epoch=[43, 81], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
+  </si>
+  <si>
+    <t>arccos margin, s=5, m=0.05, lr=0.01, decay epoch=[43, 81], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
+  </si>
+  <si>
+    <t>novoting_densenet121_ArcMargin_2020-12-29_2-7_epoch63</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-29_2-7_epoch63</t>
+  </si>
+  <si>
+    <t>arccos margin, s=5, m=0.05, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
+  </si>
+  <si>
+    <t>arccos margin, s=5, m=0.1, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-29_2-3_epoch43</t>
+  </si>
+  <si>
+    <t>novoting_densenet121_ArcMargin_2020-12-29_2-3_epoch43</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-29_18-9_epoch50</t>
+  </si>
+  <si>
+    <t>arccos margin, s=5, m=0.2, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-29_22-52_epoch46</t>
+  </si>
+  <si>
+    <t>arccos margin, s=5, m=0.15, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
+  </si>
+  <si>
+    <t>arccos margin, s=3, m=0.1, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-29_22-55_epoch57</t>
+  </si>
+  <si>
+    <t>arccos margin, s=3, m=0.1, lr=0.1, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2020-12-29_23-27_epoch82</t>
   </si>
 </sst>
 </file>
@@ -261,13 +321,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,7 +611,16 @@
                   <c:v>0.755</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.746</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.73199999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1665,7 +1734,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1744,7 @@
     <col min="3" max="3" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="13.7109375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="49.42578125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="46.5" x14ac:dyDescent="0.25">
@@ -1726,7 +1795,7 @@
       <c r="G2" s="8">
         <v>50</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="10"/>
@@ -1760,7 +1829,7 @@
       <c r="G3" s="8">
         <v>50</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="10"/>
@@ -1794,7 +1863,7 @@
       <c r="G4" s="8">
         <v>50</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="10"/>
@@ -1808,10 +1877,10 @@
     </row>
     <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="9">
         <v>44170</v>
@@ -1828,8 +1897,8 @@
       <c r="G5" s="8">
         <v>50</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>17</v>
+      <c r="H5" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -1842,10 +1911,10 @@
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="9">
         <v>44170</v>
@@ -1862,8 +1931,8 @@
       <c r="G6" s="8">
         <v>50</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>17</v>
+      <c r="H6" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -1876,10 +1945,10 @@
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="9">
         <v>44170</v>
@@ -1896,8 +1965,8 @@
       <c r="G7" s="8">
         <v>50</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>20</v>
+      <c r="H7" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -1909,27 +1978,29 @@
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="B8" s="6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C8" s="9">
-        <v>44170</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>44192</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.746</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="8">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G8" s="8">
-        <v>50</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>16</v>
+        <v>150</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -1940,10 +2011,31 @@
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
+    <row r="9" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9">
+        <v>44193</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="8">
+        <v>32</v>
+      </c>
+      <c r="G9" s="8">
+        <v>150</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -1953,10 +2045,31 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
     </row>
-    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
+    <row r="10" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="9">
+        <v>44193</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="8">
+        <v>32</v>
+      </c>
+      <c r="G10" s="8">
+        <v>150</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -1966,35 +2079,161 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
+    <row r="11" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="9">
+        <v>44194</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="8">
+        <v>32</v>
+      </c>
+      <c r="G11" s="8">
+        <v>150</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="9">
+        <v>44194</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8">
+        <v>32</v>
+      </c>
+      <c r="G12" s="8">
+        <v>150</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="9">
+        <v>44194</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="8">
+        <v>32</v>
+      </c>
+      <c r="G13" s="8">
+        <v>100</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="9">
+        <v>44195</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="8">
+        <v>32</v>
+      </c>
+      <c r="G14" s="8">
+        <v>100</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="9">
+        <v>44195</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="8">
+        <v>32</v>
+      </c>
+      <c r="G15" s="8">
+        <v>100</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="9">
+        <v>44195</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="8">
+        <v>32</v>
+      </c>
+      <c r="G16" s="8">
+        <v>100</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -2142,12 +2381,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>26</v>
+      <c r="A1" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working efficient net train script update new results and NOTES.xlsx add confusion matrix generate code remove some preprocess steps improve accuracy
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -1,32 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\code\thesisms\skinlesion\code\isic2018_lesion-diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA16A7CC-818B-4D5D-8A74-3F319A84A045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6214139-4B38-4C68-957E-A3C18576A1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="2610" windowWidth="17400" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
     <sheet name="formula note" sheetId="2" r:id="rId2"/>
+    <sheet name="note" sheetId="4" r:id="rId3"/>
+    <sheet name="number of params" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="97">
   <si>
     <t>Submissions</t>
   </si>
@@ -46,55 +58,112 @@
     <t>Voting</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>Batch size</t>
   </si>
   <si>
-    <t>novoting_full_densenet121_AutoWtdCE_2020-12-05_13-22_epoch46</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-12-05_13-22_epoch46</t>
-  </si>
-  <si>
     <t>Epoch</t>
   </si>
   <si>
-    <t>novoting_full_densenet121_AutoWtdCE_2020-12-05_13-22_epoch49</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-12-05_13-22_epoch49</t>
-  </si>
-  <si>
-    <t>bets val loss</t>
-  </si>
-  <si>
-    <t>last epoch</t>
-  </si>
-  <si>
-    <t>add random brightness, rotate, best val loss</t>
-  </si>
-  <si>
-    <t>add random brightness, rotate, last epoch</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-12-05_19-46_epoch37</t>
-  </si>
-  <si>
-    <t>voting_full_densenet121_AutoWtdCE_2020-12-05_19-46_epoch37</t>
-  </si>
-  <si>
-    <t>novoting_full_densenet121_AutoWtdCE_2020-12-05_19-46_epoch37</t>
-  </si>
-  <si>
-    <t>full_densenet121_AutoWtdCE_2020-12-05_19-46_epoch49</t>
-  </si>
-  <si>
-    <t>voting_full_densenet121_AutoWtdCE_2020-12-05_19-46_epoch49</t>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Loss layer/function</t>
+  </si>
+  <si>
+    <t>Densenet 121</t>
+  </si>
+  <si>
+    <t>Arc Cosine Margin layer + Cross Entropy</t>
+  </si>
+  <si>
+    <t>Densenet 201</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-01-06_0-59_epoch99</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-01-06_17-36_epoch99</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 decay by 0.1 every 5 epochs with stable train loss , decay epoch=[40, 80], last epoch (not working)</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 multiply by 10 every 5 epochs with stable train loss , decay epoch=[40, 80], last epoch (not working)</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increasw by 10 at epoch 60, decay epoch=[20, 30]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arccos margin weight_decay = 0.001, s=5, m=0.1 , decay epoch=[20, 30], center crop </t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-01-13_0-27_epoch99</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 , decay epoch=[20, 30], center crop, multiply by 1.5 at epoch 60</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-01-14_0-13_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1, lr=0.01, decay epoch=[20, 30], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()], no noise augment</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-01-20_23-47_epoch23</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-01-22_1-12_epoch99</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-01-23_18-49_epoch23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.3 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment</t>
+  </si>
+  <si>
+    <t>densenet201_ArcMargin_2021-03-20_13-24_epoch99</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.05 increase by 1.2 at epoch 50, lr=0.01, decay epoch=[43], no noise augment</t>
+  </si>
+  <si>
+    <t>densenet201_ArcMargin_2021-03-21_2-6_epoch99</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.05 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment</t>
+  </si>
+  <si>
+    <t>densenet201_ArcMargin_2021-03-25_0-54_epoch99</t>
+  </si>
+  <si>
+    <t>densenet201_ArcMargin_2021-03-21_20-20_epoch99</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.05 increase by 1.2 at epoch 50, lr=0.01, decay epoch=[43], no noise augment, dropout=0.2</t>
+  </si>
+  <si>
+    <t>densenet201_ArcMargin_2021-03-28_16-31_epoch99</t>
+  </si>
+  <si>
+    <t>Densenet 161</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.075 increase by 1.2 at epoch 50, lr=0.01, decay epoch=[43], no noise augment</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 50, lr=0.01, decay epoch=[43], no noise augment</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-03-31_2-36_epoch99</t>
+  </si>
+  <si>
+    <t>densenet161_ArcMargin_2021-04-01_1-20_epoch99</t>
   </si>
   <si>
     <r>
@@ -141,86 +210,207 @@
       <t xml:space="preserve">
 Here,
   - wj is the weight for each class(j signifies the class)
-  - n_samplesis the total number of samples or rows in the dataset
-  - n_classesis the total number of unique classes in the target
-  - n_samplesjis the total number of rows of the respective class</t>
+  - n_samples is the total number of samples or rows in the dataset
+  - n_classes is the total number of unique classes in the target
+  - n_samplesj is the total number of rows of the respective class</t>
     </r>
   </si>
   <si>
-    <t>novoting_densenet121_ArcMargin_2020-12-27_12-36_epoch141</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-27_12-36_epoch141</t>
-  </si>
-  <si>
-    <t>novoting_densenet121_ArcMargin_2020-12-28_0-41_epoch44</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-28_0-41_epoch44</t>
-  </si>
-  <si>
-    <t>arccos margin, s=5, m=0.05, lr=0.01, decay epoch=[43]</t>
-  </si>
-  <si>
-    <t>novoting_densenet121_ArcMargin_2020-12-28_0-36_epoch55</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-28_0-36_epoch55</t>
-  </si>
-  <si>
-    <t>arccos margin, s=5, m=0.1, lr=0.01, decay epoch=[43, 81], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
-  </si>
-  <si>
-    <t>arccos margin, s=5, m=0.05, lr=0.01, decay epoch=[43, 81], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
-  </si>
-  <si>
-    <t>novoting_densenet121_ArcMargin_2020-12-29_2-7_epoch63</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-29_2-7_epoch63</t>
-  </si>
-  <si>
-    <t>arccos margin, s=5, m=0.05, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
-  </si>
-  <si>
-    <t>arccos margin, s=5, m=0.1, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-29_2-3_epoch43</t>
-  </si>
-  <si>
-    <t>novoting_densenet121_ArcMargin_2020-12-29_2-3_epoch43</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-29_18-9_epoch50</t>
-  </si>
-  <si>
-    <t>arccos margin, s=5, m=0.2, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-29_22-52_epoch46</t>
-  </si>
-  <si>
-    <t>arccos margin, s=5, m=0.15, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
-  </si>
-  <si>
-    <t>arccos margin, s=3, m=0.1, lr=0.01, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-29_22-55_epoch57</t>
-  </si>
-  <si>
-    <t>arccos margin, s=3, m=0.1, lr=0.1, decay epoch=[43], classifier = [nn.Linear(num_ftrs, 512), nn.ReLU()]</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2020-12-29_23-27_epoch82</t>
+    <t>model</t>
+  </si>
+  <si>
+    <t>no params</t>
+  </si>
+  <si>
+    <t>input size</t>
+  </si>
+  <si>
+    <t>(300,400,3)</t>
+  </si>
+  <si>
+    <t>mbv2</t>
+  </si>
+  <si>
+    <t>densenet121</t>
+  </si>
+  <si>
+    <t>densenet201</t>
+  </si>
+  <si>
+    <t>resnet50</t>
+  </si>
+  <si>
+    <t>resnet50v2</t>
+  </si>
+  <si>
+    <t>efficientnet b0</t>
+  </si>
+  <si>
+    <t>efficientnet b1</t>
+  </si>
+  <si>
+    <t>efficientnet b2</t>
+  </si>
+  <si>
+    <t>efficientnet b3</t>
+  </si>
+  <si>
+    <t>vgg16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 not decay, lr=0.01, decay epoch=[20, 30], focal loss</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMarginFocal_2021-04-11_16-35_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 not decay, lr=0.01, decay epoch=[20, 30]</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-04-11_16-39_epoch99</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMarginFocal_2021-04-12_0-48_epoch99</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, focal loss</t>
+  </si>
+  <si>
+    <t>Arc Cosine Margin layer + Focal Loss</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-05-06_23-59_epoch90</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], random clsas weights every epoch</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], random clsas weights every iteration</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-05-09_1-29_epoch80</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-05-25_1-3_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], 90% train 10% val data</t>
+  </si>
+  <si>
+    <t>Efficientnet b0</t>
+  </si>
+  <si>
+    <t>efficientnet_b0_ArcMargin_2021-06-07_2-57_epoch99</t>
+  </si>
+  <si>
+    <t>efficientnet_b0_ArcMargin_2021-06-07_2-57_epoch67</t>
+  </si>
+  <si>
+    <t>Efficientnet b2</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-08_2-18_epoch99</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-08_2-18_epoch34</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-08_1-59_epoch95</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-08_1-59_epoch99</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-09_2-33_epoch63</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-16_0-8_epoch78</t>
+  </si>
+  <si>
+    <t>pw</t>
+  </si>
+  <si>
+    <t>pw(c-1)/(1-pw)</t>
+  </si>
+  <si>
+    <t>log()*(c-1)/c</t>
+  </si>
+  <si>
+    <t>c/(c-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test, increase crop size (random, center) by 50px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-17_2-58_epoch85</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-17_18-11_epoch80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-17_18-11_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=7, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-18_17-57_epoch60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad:
+ - dropout
+ - small batch
+ - noise augment
+ - small m for big network
+ - 
+good:
+ - center crop at testing
+ - dropout 0.2 good for efficientnet b2 (0.3 decrease results)
+try: 
+random dynamic class weights every epoch
+no samples: 10 |	 20 |	 30 |	 25	
+weights: 0.8 |	 0.6 |	 0.4 |	 0.5	
+focal+hinge loss				
+attention based		
+  params_dict = {
+      # (width_coefficient, depth_coefficient, resolution, dropout_rate)
+      'efficientnet-b0': (1.0, 1.0, 224, 0.2),
+      'efficientnet-b1': (1.0, 1.1, 240, 0.2),
+      'efficientnet-b2': (1.1, 1.2, 260, 0.3),
+      'efficientnet-b3': (1.2, 1.4, 300, 0.3),
+      'efficientnet-b4': (1.4, 1.8, 380, 0.4),
+      'efficientnet-b5': (1.6, 2.2, 456, 0.4),
+      'efficientnet-b6': (1.8, 2.6, 528, 0.5),
+      'efficientnet-b7': (2.0, 3.1, 600, 0.5),
+      'efficientnet-b8': (2.2, 3.6, 672, 0.5),
+      'efficientnet-l2': (4.3, 5.3, 800, 0.5),
+  }	</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-1010409]d\ mmm\ yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -246,13 +436,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -263,6 +446,13 @@
       <b/>
       <sz val="20"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,10 +475,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -308,32 +499,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -350,7 +561,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -588,39 +804,111 @@
           </c:dLbls>
           <c:yVal>
             <c:numRef>
-              <c:f>results!$D$2:$D$11</c:f>
+              <c:f>results!$C$2:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>0.751</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.751</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.16400000000000001</c:v>
+                  <c:v>0.72499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.755</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16700000000000001</c:v>
+                  <c:v>0.754</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.755</c:v>
+                  <c:v>0.77400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.746</c:v>
+                  <c:v>0.79100000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.72699999999999998</c:v>
+                  <c:v>0.75800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.72599999999999998</c:v>
+                  <c:v>0.75800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0.77900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.73099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.75700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.73499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.72399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.74199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.73699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.71899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.77300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>0.73199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.747</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.74399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.73699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.73399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.72499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.747</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.74099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.79300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.79100000000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.753</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,16 +1702,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>22226</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>506413</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>167482</xdr:rowOff>
+      <xdr:rowOff>195263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>29369</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1452,19 +1740,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:H41" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H41" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{D38226B5-D5DC-4676-BA69-0BF4479F00E0}" name="Date" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{6E53C4CB-4A70-41F7-B3E6-AC55510650BC}" name="Voting" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{1ABD848E-ABED-4151-A1D7-F38492E6213F}" name="Batch size" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{9E6EDDE2-5951-49F3-BEC8-6D7190A570DA}" name="Epoch" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:J50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:J50" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J50">
+    <sortCondition ref="F1:F50"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3E8B0DCA-57BB-461C-8A6E-9FA34A7B2BE6}" name="Architecture" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{87609125-158C-4CC5-AA8E-EEF050A67A7F}" name="Loss layer/function" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{E89C1E6C-8810-4E4B-B144-549BA40B4E4E}" name="Date" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{6E53C4CB-4A70-41F7-B3E6-AC55510650BC}" name="Voting" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{1ABD848E-ABED-4151-A1D7-F38492E6213F}" name="Batch size" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{9E6EDDE2-5951-49F3-BEC8-6D7190A570DA}" name="Epoch" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{52418DD9-9D63-48E7-A285-A191AA8944C9}" name="Table2" displayName="Table2" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{287206B4-2679-4CC1-86FC-2912684FA441}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
+    <sortCondition ref="B1:B11"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{BA1A0B66-9C88-496F-9F8A-5DCECE37CAF5}" name="model"/>
+    <tableColumn id="2" xr3:uid="{BB36172F-4C43-4AA6-A2BD-3C384E53BAB9}" name="no params" dataDxfId="0" dataCellStyle="Comma"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1731,23 +2038,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="44.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.7109375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="13.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="49.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1755,610 +2065,1120 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="9">
-        <v>44170</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.751</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F2" s="8">
+        <v>44202</v>
+      </c>
+      <c r="H2" s="7">
+        <v>32</v>
+      </c>
+      <c r="I2" s="7">
+        <v>100</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8">
-        <v>50</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-    </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="F3" s="8">
+        <v>44202</v>
+      </c>
+      <c r="H3" s="7">
+        <v>32</v>
+      </c>
+      <c r="I3" s="7">
+        <v>100</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="D4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="9">
-        <v>44170</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.751</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="8">
-        <v>12</v>
-      </c>
-      <c r="G3" s="8">
-        <v>50</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="9">
-        <v>44170</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="F4" s="8">
-        <v>12</v>
-      </c>
-      <c r="G4" s="8">
-        <v>50</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+        <v>44207</v>
+      </c>
+      <c r="H4" s="7">
+        <v>32</v>
+      </c>
+      <c r="I4" s="7">
+        <v>100</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9">
-        <v>44170</v>
-      </c>
-      <c r="D5" s="4">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4">
         <v>0.755</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>6</v>
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F5" s="8">
+        <v>44209</v>
+      </c>
+      <c r="H5" s="7">
+        <v>32</v>
+      </c>
+      <c r="I5" s="7">
+        <v>100</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.754</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="8">
-        <v>50</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="9">
-        <v>44170</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="F6" s="8">
+        <v>44210</v>
+      </c>
+      <c r="H6" s="7">
+        <v>32</v>
+      </c>
+      <c r="I6" s="7">
+        <v>100</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="8">
-        <v>50</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="9">
-        <v>44170</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.755</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="F7" s="8">
-        <v>12</v>
-      </c>
-      <c r="G7" s="8">
-        <v>50</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-    </row>
-    <row r="8" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44216</v>
+      </c>
+      <c r="H7" s="7">
+        <v>32</v>
+      </c>
+      <c r="I7" s="7">
+        <v>100</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="9">
-        <v>44192</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.746</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>6</v>
+      <c r="C8" s="4">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="8">
+        <v>44218</v>
+      </c>
+      <c r="H8" s="7">
         <v>32</v>
       </c>
-      <c r="G8" s="8">
-        <v>150</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-    </row>
-    <row r="9" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="7">
+        <v>100</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="9">
-        <v>44193</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.72699999999999998</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>6</v>
+        <v>26</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F9" s="8">
+        <v>44219</v>
+      </c>
+      <c r="H9" s="7">
         <v>32</v>
       </c>
-      <c r="G9" s="8">
-        <v>150</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-    </row>
-    <row r="10" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="7">
+        <v>100</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="8">
+        <v>44275</v>
+      </c>
+      <c r="H10" s="7">
+        <v>32</v>
+      </c>
+      <c r="I10" s="7">
+        <v>100</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="8">
+        <v>44276</v>
+      </c>
+      <c r="H11" s="7">
+        <v>32</v>
+      </c>
+      <c r="I11" s="7">
+        <v>100</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="9">
-        <v>44193</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="8">
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="8">
+        <v>44280</v>
+      </c>
+      <c r="H12" s="7">
+        <v>16</v>
+      </c>
+      <c r="I12" s="7">
+        <v>100</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="8">
-        <v>150</v>
-      </c>
-      <c r="H10" s="11" t="s">
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8">
+        <v>44281</v>
+      </c>
+      <c r="H13" s="7">
         <v>32</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="9">
-        <v>44194</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="I13" s="7">
+        <v>100</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="8">
+        <v>44283</v>
+      </c>
+      <c r="H14" s="7">
+        <v>32</v>
+      </c>
+      <c r="I14" s="7">
+        <v>100</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="8">
+        <v>44286</v>
+      </c>
+      <c r="H15" s="7">
+        <v>24</v>
+      </c>
+      <c r="I15" s="7">
+        <v>100</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="8">
+        <v>44287</v>
+      </c>
+      <c r="H16" s="7">
+        <v>32</v>
+      </c>
+      <c r="I16" s="7">
+        <v>100</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="8">
+        <v>44297</v>
+      </c>
+      <c r="H17" s="7">
+        <v>32</v>
+      </c>
+      <c r="I17" s="7">
+        <v>100</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="8">
+        <v>44297</v>
+      </c>
+      <c r="H18" s="7">
+        <v>32</v>
+      </c>
+      <c r="I18" s="7">
+        <v>100</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="8">
+        <v>44298</v>
+      </c>
+      <c r="H19" s="7">
+        <v>32</v>
+      </c>
+      <c r="I19" s="7">
+        <v>100</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="8">
+        <v>44325</v>
+      </c>
+      <c r="H20" s="7">
+        <v>32</v>
+      </c>
+      <c r="I20" s="7">
+        <v>100</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="8">
+        <v>44325</v>
+      </c>
+      <c r="H21" s="7">
+        <v>32</v>
+      </c>
+      <c r="I21" s="7">
+        <v>100</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="8">
+        <v>44341</v>
+      </c>
+      <c r="H22" s="7">
+        <v>32</v>
+      </c>
+      <c r="I22" s="7">
+        <v>100</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="8">
+        <v>44354</v>
+      </c>
+      <c r="H23" s="7">
+        <v>16</v>
+      </c>
+      <c r="I23" s="7">
+        <v>100</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="8">
+        <v>44354</v>
+      </c>
+      <c r="H24" s="7">
+        <v>16</v>
+      </c>
+      <c r="I24" s="7">
+        <v>100</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="4">
         <v>0.73199999999999998</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="8">
+      <c r="D25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="8">
+        <v>44354</v>
+      </c>
+      <c r="H25" s="7">
+        <v>16</v>
+      </c>
+      <c r="I25" s="7">
+        <v>100</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.747</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="8">
+        <v>44355</v>
+      </c>
+      <c r="H26" s="7">
         <v>32</v>
       </c>
-      <c r="G11" s="8">
-        <v>150</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="9">
-        <v>44194</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="I26" s="7">
+        <v>100</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="4">
         <v>0.74399999999999999</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="D27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="8">
+        <v>44355</v>
+      </c>
+      <c r="H27" s="7">
         <v>32</v>
       </c>
-      <c r="G12" s="8">
-        <v>150</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="9">
-        <v>44194</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="I27" s="7">
+        <v>100</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="8">
+        <v>44355</v>
+      </c>
+      <c r="H28" s="7">
         <v>32</v>
       </c>
-      <c r="G13" s="8">
+      <c r="I28" s="7">
         <v>100</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="9">
-        <v>44195</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="J28" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="8">
+        <v>44355</v>
+      </c>
+      <c r="H29" s="7">
         <v>32</v>
       </c>
-      <c r="G14" s="8">
+      <c r="I29" s="7">
         <v>100</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="9">
-        <v>44195</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="J29" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="8">
+        <v>44355</v>
+      </c>
+      <c r="H30" s="7">
         <v>32</v>
       </c>
-      <c r="G15" s="8">
+      <c r="I30" s="7">
         <v>100</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="9">
-        <v>44195</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="J30" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="8">
+        <v>44356</v>
+      </c>
+      <c r="H31" s="7">
         <v>32</v>
       </c>
-      <c r="G16" s="8">
+      <c r="I31" s="7">
         <v>100</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J31" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.747</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="8">
+        <v>44363</v>
+      </c>
+      <c r="H32" s="7">
+        <v>16</v>
+      </c>
+      <c r="I32" s="7">
+        <v>100</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="8">
+        <v>44364</v>
+      </c>
+      <c r="H33" s="7">
+        <v>16</v>
+      </c>
+      <c r="I33" s="7">
+        <v>100</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="8">
+        <v>44365</v>
+      </c>
+      <c r="H34" s="7">
+        <v>16</v>
+      </c>
+      <c r="I34" s="7">
+        <v>100</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="8">
+        <v>44365</v>
+      </c>
+      <c r="H35" s="7">
+        <v>16</v>
+      </c>
+      <c r="I35" s="7">
+        <v>100</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.753</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="8">
+        <v>44365</v>
+      </c>
+      <c r="H36" s="7">
+        <v>16</v>
+      </c>
+      <c r="I36" s="7">
+        <v>100</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="G49" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="G50" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2381,12 +3201,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>23</v>
+      <c r="A1" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2395,4 +3215,319 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CDDDD4-933D-499F-91EF-571E60B6B67B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1048576"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E4D789-E750-4B85-ABEB-9C7533DED1BF}">
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2257984</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="10">
+        <v>4049571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="10">
+        <v>6575239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="10">
+        <v>7037504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="10">
+        <v>7768569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="10">
+        <v>10783535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="10">
+        <v>14714688</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="10">
+        <v>18321984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="10">
+        <v>23564800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="10">
+        <v>23587712</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="10"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="10"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="10"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="10"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="10"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="10"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="10"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="10"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="10"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="10"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="10"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE87C9B-D5D6-4E07-B9D8-58CD371EBDA6}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.99999998999999995</v>
+      </c>
+      <c r="B2">
+        <f>6*A2/(1-A2)</f>
+        <v>599999990.98514438</v>
+      </c>
+      <c r="C2">
+        <f>LOG(B2)*6/7</f>
+        <v>7.5241296375929778</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>7/6</f>
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change log: - update results - remove saving state dict in train2.py - add balance_dataloader.py for balancing sampler - update new confusion matrix of new models
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\code\thesisms\skinlesion\code\isic2018_lesion-diagnosis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6214139-4B38-4C68-957E-A3C18576A1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B42C53D-6E3F-4105-8F95-903C10E44E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2610" windowWidth="17400" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="1380" windowWidth="21600" windowHeight="13335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -24,24 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="97">
-  <si>
-    <t>Submissions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="104">
   <si>
     <t>Date</t>
   </si>
@@ -357,19 +345,10 @@
     <t>efficientnet_b2_ArcMargin_2021-06-17_2-58_epoch85</t>
   </si>
   <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450</t>
-  </si>
-  <si>
     <t>efficientnet_b2_ArcMargin_2021-06-17_18-11_epoch80</t>
   </si>
   <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
-  </si>
-  <si>
     <t>efficientnet_b2_ArcMargin_2021-06-17_18-11_epoch99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=7, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
   </si>
   <si>
     <t>efficientnet_b2_ArcMargin_2021-06-18_17-57_epoch60</t>
@@ -403,6 +382,39 @@
       'efficientnet-b8': (2.2, 3.6, 672, 0.5),
       'efficientnet-l2': (4.3, 5.3, 800, 0.5),
   }	</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-19_22-45_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-08-01_3-5_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2, balance sampler 4 classes/batch</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-08-06_22-49_epoch99</t>
+  </si>
+  <si>
+    <t>s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>s=7, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>s=5, m=0.1 multiply by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2, balance sampler 7 classes/batch</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-08-07_23-34_epoch68</t>
   </si>
 </sst>
 </file>
@@ -526,7 +538,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -568,9 +580,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -804,7 +813,7 @@
           </c:dLbls>
           <c:yVal>
             <c:numRef>
-              <c:f>results!$C$2:$C$36</c:f>
+              <c:f>results!$B$2:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -1702,13 +1711,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>506413</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>195263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>71437</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>15875</xdr:rowOff>
@@ -1740,13 +1749,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:J50" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:J50" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J50">
-    <sortCondition ref="F1:F50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:I50" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I50" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I50">
+    <sortCondition ref="E1:E50"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{BC5B359A-12F2-4C79-A418-088248F95213}" name="Submissions" dataDxfId="10"/>
+  <tableColumns count="9">
     <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="8"/>
     <tableColumn id="13" xr3:uid="{3E8B0DCA-57BB-461C-8A6E-9FA34A7B2BE6}" name="Architecture" dataDxfId="7"/>
@@ -2038,1146 +2046,1105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="7" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="49.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="49.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8">
+        <v>44202</v>
+      </c>
+      <c r="G2" s="7">
+        <v>32</v>
+      </c>
+      <c r="H2" s="7">
+        <v>100</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8">
+        <v>44202</v>
+      </c>
+      <c r="G3" s="7">
+        <v>32</v>
+      </c>
+      <c r="H3" s="7">
+        <v>100</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.74</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="7" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8">
+        <v>44207</v>
+      </c>
+      <c r="G4" s="7">
+        <v>32</v>
+      </c>
+      <c r="H4" s="7">
+        <v>100</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.755</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="8">
+        <v>44209</v>
+      </c>
+      <c r="G5" s="7">
+        <v>32</v>
+      </c>
+      <c r="H5" s="7">
+        <v>100</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.754</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="8">
+        <v>44210</v>
+      </c>
+      <c r="G6" s="7">
+        <v>32</v>
+      </c>
+      <c r="H6" s="7">
+        <v>100</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="8">
+        <v>44216</v>
+      </c>
+      <c r="G7" s="7">
+        <v>32</v>
+      </c>
+      <c r="H7" s="7">
+        <v>100</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="8">
+        <v>44218</v>
+      </c>
+      <c r="G8" s="7">
+        <v>32</v>
+      </c>
+      <c r="H8" s="7">
+        <v>100</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="8">
+        <v>44219</v>
+      </c>
+      <c r="G9" s="7">
+        <v>32</v>
+      </c>
+      <c r="H9" s="7">
+        <v>100</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="8">
-        <v>44202</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="D10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="8">
+        <v>44275</v>
+      </c>
+      <c r="G10" s="7">
         <v>32</v>
       </c>
-      <c r="I2" s="7">
-        <v>100</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="H10" s="7">
+        <v>100</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="8">
+        <v>44276</v>
+      </c>
+      <c r="G11" s="7">
+        <v>32</v>
+      </c>
+      <c r="H11" s="7">
+        <v>100</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="8">
+        <v>44280</v>
+      </c>
+      <c r="G12" s="7">
+        <v>16</v>
+      </c>
+      <c r="H12" s="7">
+        <v>100</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="8">
+        <v>44281</v>
+      </c>
+      <c r="G13" s="7">
+        <v>32</v>
+      </c>
+      <c r="H13" s="7">
+        <v>100</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="8">
+        <v>44283</v>
+      </c>
+      <c r="G14" s="7">
+        <v>32</v>
+      </c>
+      <c r="H14" s="7">
+        <v>100</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="8">
+        <v>44286</v>
+      </c>
+      <c r="G15" s="7">
+        <v>24</v>
+      </c>
+      <c r="H15" s="7">
+        <v>100</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="8">
+        <v>44287</v>
+      </c>
+      <c r="G16" s="7">
+        <v>32</v>
+      </c>
+      <c r="H16" s="7">
+        <v>100</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="8">
+        <v>44297</v>
+      </c>
+      <c r="G17" s="7">
+        <v>32</v>
+      </c>
+      <c r="H17" s="7">
+        <v>100</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="8">
+        <v>44297</v>
+      </c>
+      <c r="G18" s="7">
+        <v>32</v>
+      </c>
+      <c r="H18" s="7">
+        <v>100</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="8">
+        <v>44298</v>
+      </c>
+      <c r="G19" s="7">
+        <v>32</v>
+      </c>
+      <c r="H19" s="7">
+        <v>100</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="8">
+        <v>44325</v>
+      </c>
+      <c r="G20" s="7">
+        <v>32</v>
+      </c>
+      <c r="H20" s="7">
+        <v>100</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="8">
+        <v>44325</v>
+      </c>
+      <c r="G21" s="7">
+        <v>32</v>
+      </c>
+      <c r="H21" s="7">
+        <v>100</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="8">
+        <v>44341</v>
+      </c>
+      <c r="G22" s="7">
+        <v>32</v>
+      </c>
+      <c r="H22" s="7">
+        <v>100</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="8">
+        <v>44354</v>
+      </c>
+      <c r="G23" s="7">
+        <v>16</v>
+      </c>
+      <c r="H23" s="7">
+        <v>100</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="8">
+        <v>44354</v>
+      </c>
+      <c r="G24" s="7">
+        <v>16</v>
+      </c>
+      <c r="H24" s="7">
+        <v>100</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="8">
+        <v>44354</v>
+      </c>
+      <c r="G25" s="7">
+        <v>16</v>
+      </c>
+      <c r="H25" s="7">
+        <v>100</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.747</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="8">
+        <v>44355</v>
+      </c>
+      <c r="G26" s="7">
+        <v>32</v>
+      </c>
+      <c r="H26" s="7">
+        <v>100</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="8">
+        <v>44355</v>
+      </c>
+      <c r="G27" s="7">
+        <v>32</v>
+      </c>
+      <c r="H27" s="7">
+        <v>100</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="8">
+        <v>44355</v>
+      </c>
+      <c r="G28" s="7">
+        <v>32</v>
+      </c>
+      <c r="H28" s="7">
+        <v>100</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="8">
+        <v>44355</v>
+      </c>
+      <c r="G29" s="7">
+        <v>32</v>
+      </c>
+      <c r="H29" s="7">
+        <v>100</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="8">
+        <v>44355</v>
+      </c>
+      <c r="G30" s="7">
+        <v>32</v>
+      </c>
+      <c r="H30" s="7">
+        <v>100</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="4">
         <v>0.72499999999999998</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="8">
-        <v>44202</v>
-      </c>
-      <c r="H3" s="7">
+      <c r="C31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="8">
+        <v>44356</v>
+      </c>
+      <c r="G31" s="7">
         <v>32</v>
       </c>
-      <c r="I3" s="7">
-        <v>100</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="H31" s="7">
+        <v>100</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.747</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="8">
+        <v>44363</v>
+      </c>
+      <c r="G32" s="7">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="D4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="8">
-        <v>44207</v>
-      </c>
-      <c r="H4" s="7">
-        <v>32</v>
-      </c>
-      <c r="I4" s="7">
-        <v>100</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.755</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="8">
-        <v>44209</v>
-      </c>
-      <c r="H5" s="7">
-        <v>32</v>
-      </c>
-      <c r="I5" s="7">
-        <v>100</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="H32" s="7">
+        <v>100</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="8">
+        <v>44364</v>
+      </c>
+      <c r="G33" s="7">
+        <v>16</v>
+      </c>
+      <c r="H33" s="7">
+        <v>100</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="8">
+        <v>44365</v>
+      </c>
+      <c r="G34" s="7">
+        <v>16</v>
+      </c>
+      <c r="H34" s="7">
+        <v>100</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="8">
+        <v>44365</v>
+      </c>
+      <c r="G35" s="7">
+        <v>16</v>
+      </c>
+      <c r="H35" s="7">
+        <v>100</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0.753</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="8">
+        <v>44365</v>
+      </c>
+      <c r="G36" s="7">
+        <v>16</v>
+      </c>
+      <c r="H36" s="7">
+        <v>100</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="8">
+        <v>44368</v>
+      </c>
+      <c r="G37" s="7">
+        <v>16</v>
+      </c>
+      <c r="H37" s="7">
+        <v>100</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="4">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="8">
+        <v>44409</v>
+      </c>
+      <c r="G38" s="7">
+        <v>16</v>
+      </c>
+      <c r="H38" s="7">
+        <v>100</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="4">
         <v>0.754</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="8">
-        <v>44210</v>
-      </c>
-      <c r="H6" s="7">
-        <v>32</v>
-      </c>
-      <c r="I6" s="7">
-        <v>100</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="8">
-        <v>44216</v>
-      </c>
-      <c r="H7" s="7">
-        <v>32</v>
-      </c>
-      <c r="I7" s="7">
-        <v>100</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.79100000000000004</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="8">
-        <v>44218</v>
-      </c>
-      <c r="H8" s="7">
-        <v>32</v>
-      </c>
-      <c r="I8" s="7">
-        <v>100</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="C39" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="8">
+        <v>44415</v>
+      </c>
+      <c r="G39" s="7">
+        <v>16</v>
+      </c>
+      <c r="H39" s="7">
+        <v>100</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="4">
         <v>0.75800000000000001</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="8">
-        <v>44219</v>
-      </c>
-      <c r="H9" s="7">
-        <v>32</v>
-      </c>
-      <c r="I9" s="7">
-        <v>100</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="8">
-        <v>44275</v>
-      </c>
-      <c r="H10" s="7">
-        <v>32</v>
-      </c>
-      <c r="I10" s="7">
-        <v>100</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.77900000000000003</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="8">
-        <v>44276</v>
-      </c>
-      <c r="H11" s="7">
-        <v>32</v>
-      </c>
-      <c r="I11" s="7">
-        <v>100</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0.73099999999999998</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="8">
-        <v>44280</v>
-      </c>
-      <c r="H12" s="7">
+      <c r="C40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="8">
+        <v>44416</v>
+      </c>
+      <c r="G40" s="7">
         <v>16</v>
       </c>
-      <c r="I12" s="7">
-        <v>100</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0.77</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="8">
-        <v>44281</v>
-      </c>
-      <c r="H13" s="7">
-        <v>32</v>
-      </c>
-      <c r="I13" s="7">
-        <v>100</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="8">
-        <v>44283</v>
-      </c>
-      <c r="H14" s="7">
-        <v>32</v>
-      </c>
-      <c r="I14" s="7">
-        <v>100</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.75700000000000001</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="8">
-        <v>44286</v>
-      </c>
-      <c r="H15" s="7">
-        <v>24</v>
-      </c>
-      <c r="I15" s="7">
-        <v>100</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="8">
-        <v>44287</v>
-      </c>
-      <c r="H16" s="7">
-        <v>32</v>
-      </c>
-      <c r="I16" s="7">
-        <v>100</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="8">
-        <v>44297</v>
-      </c>
-      <c r="H17" s="7">
-        <v>32</v>
-      </c>
-      <c r="I17" s="7">
-        <v>100</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="4">
-        <v>0.72399999999999998</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="8">
-        <v>44297</v>
-      </c>
-      <c r="H18" s="7">
-        <v>32</v>
-      </c>
-      <c r="I18" s="7">
-        <v>100</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0.74199999999999999</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="8">
-        <v>44298</v>
-      </c>
-      <c r="H19" s="7">
-        <v>32</v>
-      </c>
-      <c r="I19" s="7">
-        <v>100</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="8">
-        <v>44325</v>
-      </c>
-      <c r="H20" s="7">
-        <v>32</v>
-      </c>
-      <c r="I20" s="7">
-        <v>100</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="8">
-        <v>44325</v>
-      </c>
-      <c r="H21" s="7">
-        <v>32</v>
-      </c>
-      <c r="I21" s="7">
-        <v>100</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.78800000000000003</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="8">
-        <v>44341</v>
-      </c>
-      <c r="H22" s="7">
-        <v>32</v>
-      </c>
-      <c r="I22" s="7">
-        <v>100</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.77300000000000002</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="8">
-        <v>44354</v>
-      </c>
-      <c r="H23" s="7">
-        <v>16</v>
-      </c>
-      <c r="I23" s="7">
-        <v>100</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0.76</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="8">
-        <v>44354</v>
-      </c>
-      <c r="H24" s="7">
-        <v>16</v>
-      </c>
-      <c r="I24" s="7">
-        <v>100</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="8">
-        <v>44354</v>
-      </c>
-      <c r="H25" s="7">
-        <v>16</v>
-      </c>
-      <c r="I25" s="7">
-        <v>100</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="4">
-        <v>0.747</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="8">
-        <v>44355</v>
-      </c>
-      <c r="H26" s="7">
-        <v>32</v>
-      </c>
-      <c r="I26" s="7">
-        <v>100</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="8">
-        <v>44355</v>
-      </c>
-      <c r="H27" s="7">
-        <v>32</v>
-      </c>
-      <c r="I27" s="7">
-        <v>100</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="8">
-        <v>44355</v>
-      </c>
-      <c r="H28" s="7">
-        <v>32</v>
-      </c>
-      <c r="I28" s="7">
-        <v>100</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="4">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="8">
-        <v>44355</v>
-      </c>
-      <c r="H29" s="7">
-        <v>32</v>
-      </c>
-      <c r="I29" s="7">
-        <v>100</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="4">
-        <v>0.73</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="8">
-        <v>44355</v>
-      </c>
-      <c r="H30" s="7">
-        <v>32</v>
-      </c>
-      <c r="I30" s="7">
-        <v>100</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="8">
-        <v>44356</v>
-      </c>
-      <c r="H31" s="7">
-        <v>32</v>
-      </c>
-      <c r="I31" s="7">
-        <v>100</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0.747</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="8">
-        <v>44363</v>
-      </c>
-      <c r="H32" s="7">
-        <v>16</v>
-      </c>
-      <c r="I32" s="7">
-        <v>100</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="4">
-        <v>0.74099999999999999</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="8">
-        <v>44364</v>
-      </c>
-      <c r="H33" s="7">
-        <v>16</v>
-      </c>
-      <c r="I33" s="7">
-        <v>100</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="4">
-        <v>0.79300000000000004</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="8">
-        <v>44365</v>
-      </c>
-      <c r="H34" s="7">
-        <v>16</v>
-      </c>
-      <c r="I34" s="7">
-        <v>100</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0.79100000000000004</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="8">
-        <v>44365</v>
-      </c>
-      <c r="H35" s="7">
-        <v>16</v>
-      </c>
-      <c r="I35" s="7">
-        <v>100</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="4">
-        <v>0.753</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="8">
-        <v>44365</v>
-      </c>
-      <c r="H36" s="7">
-        <v>16</v>
-      </c>
-      <c r="I36" s="7">
-        <v>100</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H40" s="7">
+        <v>100</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="G49" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F49" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="G50" s="7" t="s">
-        <v>6</v>
+      <c r="F50" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3206,7 +3173,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3232,7 +3199,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3260,29 +3227,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="10">
         <v>2257984</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="10">
         <v>4049571</v>
@@ -3290,7 +3257,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="10">
         <v>6575239</v>
@@ -3298,7 +3265,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="10">
         <v>7037504</v>
@@ -3306,7 +3273,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="10">
         <v>7768569</v>
@@ -3314,7 +3281,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="10">
         <v>10783535</v>
@@ -3322,7 +3289,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="10">
         <v>14714688</v>
@@ -3330,7 +3297,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="10">
         <v>18321984</v>
@@ -3338,7 +3305,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="10">
         <v>23564800</v>
@@ -3346,7 +3313,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="10">
         <v>23587712</v>
@@ -3494,13 +3461,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>81</v>
-      </c>
-      <c r="C1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3518,7 +3485,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change log: - update result of auto margin
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B42C53D-6E3F-4105-8F95-903C10E44E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DF08CA-4A48-48A4-B2DD-E931D6AEF4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1380" windowWidth="21600" windowHeight="13335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="107">
   <si>
     <t>Date</t>
   </si>
@@ -152,6 +152,228 @@
   </si>
   <si>
     <t>densenet161_ArcMargin_2021-04-01_1-20_epoch99</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>no params</t>
+  </si>
+  <si>
+    <t>input size</t>
+  </si>
+  <si>
+    <t>(300,400,3)</t>
+  </si>
+  <si>
+    <t>mbv2</t>
+  </si>
+  <si>
+    <t>densenet121</t>
+  </si>
+  <si>
+    <t>densenet201</t>
+  </si>
+  <si>
+    <t>resnet50</t>
+  </si>
+  <si>
+    <t>resnet50v2</t>
+  </si>
+  <si>
+    <t>efficientnet b0</t>
+  </si>
+  <si>
+    <t>efficientnet b1</t>
+  </si>
+  <si>
+    <t>efficientnet b2</t>
+  </si>
+  <si>
+    <t>efficientnet b3</t>
+  </si>
+  <si>
+    <t>vgg16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 not decay, lr=0.01, decay epoch=[20, 30], focal loss</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMarginFocal_2021-04-11_16-35_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 not decay, lr=0.01, decay epoch=[20, 30]</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-04-11_16-39_epoch99</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMarginFocal_2021-04-12_0-48_epoch99</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, focal loss</t>
+  </si>
+  <si>
+    <t>Arc Cosine Margin layer + Focal Loss</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-05-06_23-59_epoch90</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], random clsas weights every epoch</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], random clsas weights every iteration</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-05-09_1-29_epoch80</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-05-25_1-3_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], 90% train 10% val data</t>
+  </si>
+  <si>
+    <t>Efficientnet b0</t>
+  </si>
+  <si>
+    <t>efficientnet_b0_ArcMargin_2021-06-07_2-57_epoch99</t>
+  </si>
+  <si>
+    <t>efficientnet_b0_ArcMargin_2021-06-07_2-57_epoch67</t>
+  </si>
+  <si>
+    <t>Efficientnet b2</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-08_2-18_epoch99</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-08_2-18_epoch34</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-08_1-59_epoch95</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-08_1-59_epoch99</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-09_2-33_epoch63</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-16_0-8_epoch78</t>
+  </si>
+  <si>
+    <t>pw</t>
+  </si>
+  <si>
+    <t>pw(c-1)/(1-pw)</t>
+  </si>
+  <si>
+    <t>log()*(c-1)/c</t>
+  </si>
+  <si>
+    <t>c/(c-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test, increase crop size (random, center) by 50px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-17_2-58_epoch85</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-17_18-11_epoch80</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-17_18-11_epoch99</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-18_17-57_epoch60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad:
+ - dropout
+ - small batch
+ - noise augment
+ - small m for big network
+ - 
+good:
+ - center crop at testing
+ - dropout 0.2 good for efficientnet b2 (0.3 decrease results)
+try: 
+random dynamic class weights every epoch
+no samples: 10 |	 20 |	 30 |	 25	
+weights: 0.8 |	 0.6 |	 0.4 |	 0.5	
+focal+hinge loss				
+attention based		
+  params_dict = {
+      # (width_coefficient, depth_coefficient, resolution, dropout_rate)
+      'efficientnet-b0': (1.0, 1.0, 224, 0.2),
+      'efficientnet-b1': (1.0, 1.1, 240, 0.2),
+      'efficientnet-b2': (1.1, 1.2, 260, 0.3),
+      'efficientnet-b3': (1.2, 1.4, 300, 0.3),
+      'efficientnet-b4': (1.4, 1.8, 380, 0.4),
+      'efficientnet-b5': (1.6, 2.2, 456, 0.4),
+      'efficientnet-b6': (1.8, 2.6, 528, 0.5),
+      'efficientnet-b7': (2.0, 3.1, 600, 0.5),
+      'efficientnet-b8': (2.2, 3.6, 672, 0.5),
+      'efficientnet-l2': (4.3, 5.3, 800, 0.5),
+  }	</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-06-19_22-45_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-08-01_3-5_epoch99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2, balance sampler 4 classes/batch</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-08-06_22-49_epoch99</t>
+  </si>
+  <si>
+    <t>s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>s=7, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>s=5, m=0.1 multiply by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
+  </si>
+  <si>
+    <t>s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2, balance sampler 7 classes/batch</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-08-07_23-34_epoch68</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-08-22_19-26_epoch99</t>
+  </si>
+  <si>
+    <t>Arc Cosine Auto Margin layer + Cross Entropy</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, lr=0.01, decay epoch=[20, 30], centercrop test, crop 350x450, auto margin during training</t>
   </si>
   <si>
     <r>
@@ -200,221 +422,10 @@
   - wj is the weight for each class(j signifies the class)
   - n_samples is the total number of samples or rows in the dataset
   - n_classes is the total number of unique classes in the target
-  - n_samplesj is the total number of rows of the respective class</t>
+  - n_samplesj is the total number of rows of the respective class
+Auto margin:
+ - used a simple 3 layers CNN with batch of images as input to generate average m for arc cosine margin layer</t>
     </r>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>no params</t>
-  </si>
-  <si>
-    <t>input size</t>
-  </si>
-  <si>
-    <t>(300,400,3)</t>
-  </si>
-  <si>
-    <t>mbv2</t>
-  </si>
-  <si>
-    <t>densenet121</t>
-  </si>
-  <si>
-    <t>densenet201</t>
-  </si>
-  <si>
-    <t>resnet50</t>
-  </si>
-  <si>
-    <t>resnet50v2</t>
-  </si>
-  <si>
-    <t>efficientnet b0</t>
-  </si>
-  <si>
-    <t>efficientnet b1</t>
-  </si>
-  <si>
-    <t>efficientnet b2</t>
-  </si>
-  <si>
-    <t>efficientnet b3</t>
-  </si>
-  <si>
-    <t>vgg16</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 not decay, lr=0.01, decay epoch=[20, 30], focal loss</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMarginFocal_2021-04-11_16-35_epoch99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 not decay, lr=0.01, decay epoch=[20, 30]</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2021-04-11_16-39_epoch99</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMarginFocal_2021-04-12_0-48_epoch99</t>
-  </si>
-  <si>
-    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, focal loss</t>
-  </si>
-  <si>
-    <t>Arc Cosine Margin layer + Focal Loss</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2021-05-06_23-59_epoch90</t>
-  </si>
-  <si>
-    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], random clsas weights every epoch</t>
-  </si>
-  <si>
-    <t>arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], random clsas weights every iteration</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2021-05-09_1-29_epoch80</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2021-05-25_1-3_epoch99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], 90% train 10% val data</t>
-  </si>
-  <si>
-    <t>Efficientnet b0</t>
-  </si>
-  <si>
-    <t>efficientnet_b0_ArcMargin_2021-06-07_2-57_epoch99</t>
-  </si>
-  <si>
-    <t>efficientnet_b0_ArcMargin_2021-06-07_2-57_epoch67</t>
-  </si>
-  <si>
-    <t>Efficientnet b2</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-08_2-18_epoch99</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-08_2-18_epoch34</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-08_1-59_epoch95</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-08_1-59_epoch99</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-09_2-33_epoch63</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-16_0-8_epoch78</t>
-  </si>
-  <si>
-    <t>pw</t>
-  </si>
-  <si>
-    <t>pw(c-1)/(1-pw)</t>
-  </si>
-  <si>
-    <t>log()*(c-1)/c</t>
-  </si>
-  <si>
-    <t>c/(c-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 increase by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], no noise augment, centercrop test, increase crop size (random, center) by 50px</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=3, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-17_2-58_epoch85</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-17_18-11_epoch80</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-17_18-11_epoch99</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-18_17-57_epoch60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bad:
- - dropout
- - small batch
- - noise augment
- - small m for big network
- - 
-good:
- - center crop at testing
- - dropout 0.2 good for efficientnet b2 (0.3 decrease results)
-try: 
-random dynamic class weights every epoch
-no samples: 10 |	 20 |	 30 |	 25	
-weights: 0.8 |	 0.6 |	 0.4 |	 0.5	
-focal+hinge loss				
-attention based		
-  params_dict = {
-      # (width_coefficient, depth_coefficient, resolution, dropout_rate)
-      'efficientnet-b0': (1.0, 1.0, 224, 0.2),
-      'efficientnet-b1': (1.0, 1.1, 240, 0.2),
-      'efficientnet-b2': (1.1, 1.2, 260, 0.3),
-      'efficientnet-b3': (1.2, 1.4, 300, 0.3),
-      'efficientnet-b4': (1.4, 1.8, 380, 0.4),
-      'efficientnet-b5': (1.6, 2.2, 456, 0.4),
-      'efficientnet-b6': (1.8, 2.6, 528, 0.5),
-      'efficientnet-b7': (2.0, 3.1, 600, 0.5),
-      'efficientnet-b8': (2.2, 3.6, 672, 0.5),
-      'efficientnet-l2': (4.3, 5.3, 800, 0.5),
-  }	</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-06-19_22-45_epoch99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-08-01_3-5_epoch99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2, balance sampler 4 classes/batch</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-08-06_22-49_epoch99</t>
-  </si>
-  <si>
-    <t>s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
-  </si>
-  <si>
-    <t>s=7, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
-  </si>
-  <si>
-    <t>s=5, m=0.1 multiply by 1.2 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2</t>
-  </si>
-  <si>
-    <t>s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arccos margin weight_decay = 0.001, s=5, m=0.05 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2, balance sampler 7 classes/batch</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-08-07_23-34_epoch68</t>
   </si>
 </sst>
 </file>
@@ -2048,8 +2059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,7 +2491,7 @@
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="4">
         <v>0.75800000000000001</v>
@@ -2489,7 +2500,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="8">
         <v>44297</v>
@@ -2501,12 +2512,12 @@
         <v>100</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="4">
         <v>0.72399999999999998</v>
@@ -2527,12 +2538,12 @@
         <v>100</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4">
         <v>0.74199999999999999</v>
@@ -2541,7 +2552,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" s="8">
         <v>44298</v>
@@ -2553,12 +2564,12 @@
         <v>100</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="4">
         <v>0.73699999999999999</v>
@@ -2579,12 +2590,12 @@
         <v>100</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="4">
         <v>0.71899999999999997</v>
@@ -2605,12 +2616,12 @@
         <v>100</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="4">
         <v>0.78800000000000003</v>
@@ -2631,18 +2642,18 @@
         <v>100</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="4">
         <v>0.77300000000000002</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>11</v>
@@ -2657,18 +2668,18 @@
         <v>100</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="4">
         <v>0.76</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>11</v>
@@ -2683,18 +2694,18 @@
         <v>100</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="4">
         <v>0.73199999999999998</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>11</v>
@@ -2709,18 +2720,18 @@
         <v>100</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="4">
         <v>0.747</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>11</v>
@@ -2735,18 +2746,18 @@
         <v>100</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="4">
         <v>0.74399999999999999</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>11</v>
@@ -2761,18 +2772,18 @@
         <v>100</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="4">
         <v>0.73699999999999999</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>11</v>
@@ -2787,18 +2798,18 @@
         <v>100</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="4">
         <v>0.73399999999999999</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>11</v>
@@ -2813,18 +2824,18 @@
         <v>100</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="4">
         <v>0.73</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>11</v>
@@ -2839,18 +2850,18 @@
         <v>100</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="4">
         <v>0.72499999999999998</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>11</v>
@@ -2865,18 +2876,18 @@
         <v>100</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="4">
         <v>0.747</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>11</v>
@@ -2891,18 +2902,18 @@
         <v>100</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" s="4">
         <v>0.74099999999999999</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>11</v>
@@ -2917,18 +2928,18 @@
         <v>100</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B34" s="4">
         <v>0.79300000000000004</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>11</v>
@@ -2943,18 +2954,18 @@
         <v>100</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" s="4">
         <v>0.79100000000000004</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>11</v>
@@ -2969,18 +2980,18 @@
         <v>100</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36" s="4">
         <v>0.753</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>11</v>
@@ -2995,18 +3006,18 @@
         <v>100</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="4">
         <v>0.72699999999999998</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>11</v>
@@ -3021,18 +3032,18 @@
         <v>100</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="4">
         <v>0.52800000000000002</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>11</v>
@@ -3047,18 +3058,18 @@
         <v>100</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" s="4">
         <v>0.754</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>11</v>
@@ -3073,18 +3084,18 @@
         <v>100</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="4">
         <v>0.75800000000000001</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>11</v>
@@ -3099,14 +3110,34 @@
         <v>100</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="5"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="8">
+        <v>44431</v>
+      </c>
+      <c r="G41" s="7">
+        <v>16</v>
+      </c>
+      <c r="H41" s="7">
+        <v>100</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
@@ -3162,7 +3193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEC87F6-42EF-4C28-A44C-D458D6A8AE94}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3173,7 +3204,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3199,7 +3230,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3227,29 +3258,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="10">
         <v>2257984</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="10">
         <v>4049571</v>
@@ -3257,7 +3288,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="10">
         <v>6575239</v>
@@ -3265,7 +3296,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="10">
         <v>7037504</v>
@@ -3273,7 +3304,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="10">
         <v>7768569</v>
@@ -3281,7 +3312,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="10">
         <v>10783535</v>
@@ -3289,7 +3320,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="10">
         <v>14714688</v>
@@ -3297,7 +3328,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="10">
         <v>18321984</v>
@@ -3305,7 +3336,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="10">
         <v>23564800</v>
@@ -3313,7 +3344,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="10">
         <v>23587712</v>
@@ -3461,13 +3492,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3485,7 +3516,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
remove redundant codes update new submissions, results, confusion matrix add vision transformer training and testing scripts
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DF08CA-4A48-48A4-B2DD-E931D6AEF4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2525E13-0DCD-4D60-8BA2-22AD6F076E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
   <si>
     <t>Date</t>
   </si>
@@ -302,36 +302,6 @@
   </si>
   <si>
     <t>efficientnet_b2_ArcMargin_2021-06-18_17-57_epoch60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bad:
- - dropout
- - small batch
- - noise augment
- - small m for big network
- - 
-good:
- - center crop at testing
- - dropout 0.2 good for efficientnet b2 (0.3 decrease results)
-try: 
-random dynamic class weights every epoch
-no samples: 10 |	 20 |	 30 |	 25	
-weights: 0.8 |	 0.6 |	 0.4 |	 0.5	
-focal+hinge loss				
-attention based		
-  params_dict = {
-      # (width_coefficient, depth_coefficient, resolution, dropout_rate)
-      'efficientnet-b0': (1.0, 1.0, 224, 0.2),
-      'efficientnet-b1': (1.0, 1.1, 240, 0.2),
-      'efficientnet-b2': (1.1, 1.2, 260, 0.3),
-      'efficientnet-b3': (1.2, 1.4, 300, 0.3),
-      'efficientnet-b4': (1.4, 1.8, 380, 0.4),
-      'efficientnet-b5': (1.6, 2.2, 456, 0.4),
-      'efficientnet-b6': (1.8, 2.6, 528, 0.5),
-      'efficientnet-b7': (2.0, 3.1, 600, 0.5),
-      'efficientnet-b8': (2.2, 3.6, 672, 0.5),
-      'efficientnet-l2': (4.3, 5.3, 800, 0.5),
-  }	</t>
   </si>
   <si>
     <t>efficientnet_b2_ArcMargin_2021-06-19_22-45_epoch99</t>
@@ -426,6 +396,57 @@
 Auto margin:
  - used a simple 3 layers CNN with batch of images as input to generate average m for arc cosine margin layer</t>
     </r>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, lr=0.01, decay epoch=[20, 30], centercrop test, crop 350x450, auto margin during training, focal loss</t>
+  </si>
+  <si>
+    <t>Arc Cosine Auto Margin layer + Focal Loss</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-09-03_1-7_epoch98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad:
+ - dropout
+ - small batch
+ - noise augment
+ - small m for big network
+ - 
+good:
+ - center crop at testing
+ - dropout 0.2 good for efficientnet b2 (0.3 decrease results)
+try: 
+random dynamic class weights every epoch
+no samples: 10 |	 20 |	 30 |	 25	
+weights: 0.8 |	 0.6 |	 0.4 |	 0.5	
+focal+hinge loss				
+attention based		
+  params_dict = {
+      # (width_coefficient, depth_coefficient, resolution, dropout_rate)
+      'efficientnet-b0': (1.0, 1.0, 224, 0.2),
+      'efficientnet-b1': (1.0, 1.1, 240, 0.2),
+      'efficientnet-b2': (1.1, 1.2, 260, 0.3),
+      'efficientnet-b3': (1.2, 1.4, 300, 0.3),
+      'efficientnet-b4': (1.4, 1.8, 380, 0.4),
+      'efficientnet-b5': (1.6, 2.2, 456, 0.4),
+      'efficientnet-b6': (1.8, 2.6, 528, 0.5),
+      'efficientnet-b7': (2.0, 3.1, 600, 0.5),
+      'efficientnet-b8': (2.2, 3.6, 672, 0.5),
+      'efficientnet-l2': (4.3, 5.3, 800, 0.5),
+  }	</t>
+  </si>
+  <si>
+    <t>densenet121_ArcMargin_2021-08-24_21-45_epoch32</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, lr=0.01, decay epoch=[20, 30], centercrop test, crop 350x450, auto margin + scale during training</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, lr=0.01, decay epoch=[20, 30], centercrop test, crop 350x450, auto margin during training, dropout=0.2</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-09-06_1-51_epoch99</t>
   </si>
 </sst>
 </file>
@@ -502,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -514,9 +535,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1760,10 +1778,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:I50" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:I50" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I50">
-    <sortCondition ref="E1:E50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:I51" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I51" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I51">
+    <sortCondition ref="E1:E51"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="9"/>
@@ -2057,10 +2075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,9 +2088,9 @@
     <col min="3" max="3" width="25.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" style="4" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="7" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="13.7109375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="49.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="49.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="46.5" x14ac:dyDescent="0.25">
@@ -2105,1076 +2123,1142 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="4">
         <v>0.74</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>44202</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>32</v>
       </c>
-      <c r="H2" s="7">
-        <v>100</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="6">
+        <v>100</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4">
         <v>0.72499999999999998</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>44202</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>32</v>
       </c>
-      <c r="H3" s="7">
-        <v>100</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="H3" s="6">
+        <v>100</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="A4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>44207</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>32</v>
       </c>
-      <c r="H4" s="7">
-        <v>100</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="6">
+        <v>100</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="4">
         <v>0.755</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>44209</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>32</v>
       </c>
-      <c r="H5" s="7">
-        <v>100</v>
-      </c>
-      <c r="I5" s="9" t="s">
+      <c r="H5" s="6">
+        <v>100</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="4">
         <v>0.754</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>44210</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>32</v>
       </c>
-      <c r="H6" s="7">
-        <v>100</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="H6" s="6">
+        <v>100</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="4">
         <v>0.77400000000000002</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>44216</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>32</v>
       </c>
-      <c r="H7" s="7">
-        <v>100</v>
-      </c>
-      <c r="I7" s="9" t="s">
+      <c r="H7" s="6">
+        <v>100</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4">
         <v>0.79100000000000004</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>44218</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>32</v>
       </c>
-      <c r="H8" s="7">
-        <v>100</v>
-      </c>
-      <c r="I8" s="9" t="s">
+      <c r="H8" s="6">
+        <v>100</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="4">
         <v>0.75800000000000001</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>44219</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>32</v>
       </c>
-      <c r="H9" s="7">
-        <v>100</v>
-      </c>
-      <c r="I9" s="9" t="s">
+      <c r="H9" s="6">
+        <v>100</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="4">
         <v>0.75800000000000001</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>44275</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>32</v>
       </c>
-      <c r="H10" s="7">
-        <v>100</v>
-      </c>
-      <c r="I10" s="9" t="s">
+      <c r="H10" s="6">
+        <v>100</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="4">
         <v>0.77900000000000003</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>44276</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>32</v>
       </c>
-      <c r="H11" s="7">
-        <v>100</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="H11" s="6">
+        <v>100</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="4">
         <v>0.73099999999999998</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>44280</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>16</v>
       </c>
-      <c r="H12" s="7">
-        <v>100</v>
-      </c>
-      <c r="I12" s="9" t="s">
+      <c r="H12" s="6">
+        <v>100</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="4">
         <v>0.77</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>44281</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>32</v>
       </c>
-      <c r="H13" s="7">
-        <v>100</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="H13" s="6">
+        <v>100</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="4">
         <v>0.75900000000000001</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>44283</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>32</v>
       </c>
-      <c r="H14" s="7">
-        <v>100</v>
-      </c>
-      <c r="I14" s="9" t="s">
+      <c r="H14" s="6">
+        <v>100</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="4">
         <v>0.75700000000000001</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>44286</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>24</v>
       </c>
-      <c r="H15" s="7">
-        <v>100</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="H15" s="6">
+        <v>100</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="4">
         <v>0.73499999999999999</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>44287</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>32</v>
       </c>
-      <c r="H16" s="7">
-        <v>100</v>
-      </c>
-      <c r="I16" s="9" t="s">
+      <c r="H16" s="6">
+        <v>100</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B17" s="4">
         <v>0.75800000000000001</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>44297</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>32</v>
       </c>
-      <c r="H17" s="7">
-        <v>100</v>
-      </c>
-      <c r="I17" s="9" t="s">
+      <c r="H17" s="6">
+        <v>100</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="4">
         <v>0.72399999999999998</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>44297</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>32</v>
       </c>
-      <c r="H18" s="7">
-        <v>100</v>
-      </c>
-      <c r="I18" s="9" t="s">
+      <c r="H18" s="6">
+        <v>100</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="4">
         <v>0.74199999999999999</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>44298</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>32</v>
       </c>
-      <c r="H19" s="7">
-        <v>100</v>
-      </c>
-      <c r="I19" s="9" t="s">
+      <c r="H19" s="6">
+        <v>100</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="4">
         <v>0.73699999999999999</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>44325</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>32</v>
       </c>
-      <c r="H20" s="7">
-        <v>100</v>
-      </c>
-      <c r="I20" s="9" t="s">
+      <c r="H20" s="6">
+        <v>100</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B21" s="4">
         <v>0.71899999999999997</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>44325</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>32</v>
       </c>
-      <c r="H21" s="7">
-        <v>100</v>
-      </c>
-      <c r="I21" s="9" t="s">
+      <c r="H21" s="6">
+        <v>100</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="4">
         <v>0.78800000000000003</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <v>44341</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>32</v>
       </c>
-      <c r="H22" s="7">
-        <v>100</v>
-      </c>
-      <c r="I22" s="9" t="s">
+      <c r="H22" s="6">
+        <v>100</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="4">
         <v>0.77300000000000002</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>44354</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>16</v>
       </c>
-      <c r="H23" s="7">
-        <v>100</v>
-      </c>
-      <c r="I23" s="9" t="s">
+      <c r="H23" s="6">
+        <v>100</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="4">
         <v>0.76</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>44354</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>16</v>
       </c>
-      <c r="H24" s="7">
-        <v>100</v>
-      </c>
-      <c r="I24" s="9" t="s">
+      <c r="H24" s="6">
+        <v>100</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B25" s="4">
         <v>0.73199999999999998</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <v>44354</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>16</v>
       </c>
-      <c r="H25" s="7">
-        <v>100</v>
-      </c>
-      <c r="I25" s="9" t="s">
+      <c r="H25" s="6">
+        <v>100</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="4">
         <v>0.747</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <v>44355</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>32</v>
       </c>
-      <c r="H26" s="7">
-        <v>100</v>
-      </c>
-      <c r="I26" s="9" t="s">
+      <c r="H26" s="6">
+        <v>100</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="4">
         <v>0.74399999999999999</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <v>44355</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>32</v>
       </c>
-      <c r="H27" s="7">
-        <v>100</v>
-      </c>
-      <c r="I27" s="9" t="s">
+      <c r="H27" s="6">
+        <v>100</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="4">
         <v>0.73699999999999999</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="7">
         <v>44355</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>32</v>
       </c>
-      <c r="H28" s="7">
-        <v>100</v>
-      </c>
-      <c r="I28" s="9" t="s">
+      <c r="H28" s="6">
+        <v>100</v>
+      </c>
+      <c r="I28" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B29" s="4">
         <v>0.73399999999999999</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="7">
         <v>44355</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>32</v>
       </c>
-      <c r="H29" s="7">
-        <v>100</v>
-      </c>
-      <c r="I29" s="9" t="s">
+      <c r="H29" s="6">
+        <v>100</v>
+      </c>
+      <c r="I29" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B30" s="4">
         <v>0.73</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="7">
         <v>44355</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="6">
         <v>32</v>
       </c>
-      <c r="H30" s="7">
-        <v>100</v>
-      </c>
-      <c r="I30" s="9" t="s">
+      <c r="H30" s="6">
+        <v>100</v>
+      </c>
+      <c r="I30" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B31" s="4">
         <v>0.72499999999999998</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="7">
         <v>44356</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>32</v>
       </c>
-      <c r="H31" s="7">
-        <v>100</v>
-      </c>
-      <c r="I31" s="9" t="s">
+      <c r="H31" s="6">
+        <v>100</v>
+      </c>
+      <c r="I31" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B32" s="4">
         <v>0.747</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <v>44363</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="6">
         <v>16</v>
       </c>
-      <c r="H32" s="7">
-        <v>100</v>
-      </c>
-      <c r="I32" s="9" t="s">
+      <c r="H32" s="6">
+        <v>100</v>
+      </c>
+      <c r="I32" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B33" s="4">
         <v>0.74099999999999999</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <v>44364</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="6">
         <v>16</v>
       </c>
-      <c r="H33" s="7">
-        <v>100</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>100</v>
+      <c r="H33" s="6">
+        <v>100</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="4">
         <v>0.79300000000000004</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="7">
         <v>44365</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <v>16</v>
       </c>
-      <c r="H34" s="7">
-        <v>100</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>97</v>
+      <c r="H34" s="6">
+        <v>100</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B35" s="4">
         <v>0.79100000000000004</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="7">
         <v>44365</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="6">
         <v>16</v>
       </c>
-      <c r="H35" s="7">
-        <v>100</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>97</v>
+      <c r="H35" s="6">
+        <v>100</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B36" s="4">
         <v>0.753</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="7">
         <v>44365</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="6">
         <v>16</v>
       </c>
-      <c r="H36" s="7">
-        <v>100</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>98</v>
+      <c r="H36" s="6">
+        <v>100</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>92</v>
+      <c r="A37" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="B37" s="4">
         <v>0.72699999999999998</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="7">
         <v>44368</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="6">
         <v>16</v>
       </c>
-      <c r="H37" s="7">
-        <v>100</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>99</v>
+      <c r="H37" s="6">
+        <v>100</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>94</v>
+      <c r="A38" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="B38" s="4">
         <v>0.52800000000000002</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="7">
         <v>44409</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="6">
         <v>16</v>
       </c>
-      <c r="H38" s="7">
-        <v>100</v>
-      </c>
-      <c r="I38" s="9" t="s">
+      <c r="H38" s="6">
+        <v>100</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="B39" s="4">
         <v>0.754</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="7">
         <v>44415</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="6">
         <v>16</v>
       </c>
-      <c r="H39" s="7">
-        <v>100</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>93</v>
+      <c r="H39" s="6">
+        <v>100</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>102</v>
+      <c r="A40" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="B40" s="4">
         <v>0.75800000000000001</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="7">
         <v>44416</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="6">
         <v>16</v>
       </c>
-      <c r="H40" s="7">
-        <v>100</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>101</v>
+      <c r="H40" s="6">
+        <v>100</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>103</v>
+      <c r="A41" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="B41" s="4">
         <v>0.75800000000000001</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="7">
+        <v>44431</v>
+      </c>
+      <c r="G41" s="6">
+        <v>16</v>
+      </c>
+      <c r="H41" s="6">
+        <v>100</v>
+      </c>
+      <c r="I41" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E41" s="8">
-        <v>44431</v>
-      </c>
-      <c r="G41" s="7">
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="7">
+        <v>44432</v>
+      </c>
+      <c r="G42" s="6">
         <v>16</v>
       </c>
-      <c r="H41" s="7">
-        <v>100</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="H42" s="6">
+        <v>100</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="7">
+        <v>44443</v>
+      </c>
+      <c r="G43" s="6">
+        <v>16</v>
+      </c>
+      <c r="H43" s="6">
+        <v>100</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.751</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="7">
+        <v>44445</v>
+      </c>
+      <c r="G44" s="6">
+        <v>16</v>
+      </c>
+      <c r="H44" s="6">
+        <v>100</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="A45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="A46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="A47" s="5"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="5"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="F49" s="7" t="s">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="F50" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="F50" s="7" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="F51" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3193,18 +3277,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEC87F6-42EF-4C28-A44C-D458D6A8AE94}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>106</v>
+      <c r="A1" s="10" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3225,12 +3309,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>91</v>
+      <c r="A1" s="12" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3271,7 +3355,7 @@
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>2257984</v>
       </c>
       <c r="C2" t="s">
@@ -3282,7 +3366,7 @@
       <c r="A3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>4049571</v>
       </c>
     </row>
@@ -3290,7 +3374,7 @@
       <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>6575239</v>
       </c>
     </row>
@@ -3298,7 +3382,7 @@
       <c r="A5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>7037504</v>
       </c>
     </row>
@@ -3306,7 +3390,7 @@
       <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>7768569</v>
       </c>
     </row>
@@ -3314,7 +3398,7 @@
       <c r="A7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>10783535</v>
       </c>
     </row>
@@ -3322,7 +3406,7 @@
       <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>14714688</v>
       </c>
     </row>
@@ -3330,7 +3414,7 @@
       <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>18321984</v>
       </c>
     </row>
@@ -3338,7 +3422,7 @@
       <c r="A10" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>23564800</v>
       </c>
     </row>
@@ -3346,126 +3430,126 @@
       <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>23587712</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
+      <c r="B14" s="9"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
+      <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="9"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="9"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="B18" s="9"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
+      <c r="B19" s="9"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="B20" s="9"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
+      <c r="B21" s="9"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="9"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
+      <c r="B23" s="9"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
+      <c r="B24" s="9"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
+      <c r="B25" s="9"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
+      <c r="B26" s="9"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
+      <c r="B29" s="9"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
+      <c r="B30" s="9"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
+      <c r="B31" s="9"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
+      <c r="B32" s="9"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
+      <c r="B33" s="9"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
+      <c r="B34" s="9"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
+      <c r="B35" s="9"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
+      <c r="B36" s="9"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
+      <c r="B38" s="9"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
+      <c r="B39" s="9"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
+      <c r="B40" s="9"/>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
+      <c r="B42" s="9"/>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
+      <c r="B43" s="9"/>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="10"/>
+      <c r="B44" s="9"/>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
+      <c r="B45" s="9"/>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
+      <c r="B46" s="9"/>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
+      <c r="B47" s="9"/>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="10"/>
+      <c r="B48" s="9"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
+      <c r="B49" s="9"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="10"/>
+      <c r="B50" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update new result test stock random augmentation training with efficientnet b2 crop 450x450
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2525E13-0DCD-4D60-8BA2-22AD6F076E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F6BF8-94D8-44CA-B2D0-44B72B20EDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,26 @@
     <sheet name="note" sheetId="4" r:id="rId3"/>
     <sheet name="number of params" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="low cost augmentation" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="161">
   <si>
     <t>Date</t>
   </si>
@@ -407,6 +415,18 @@
     <t>densenet121_ArcMargin_2021-09-03_1-7_epoch98</t>
   </si>
   <si>
+    <t>densenet121_ArcMargin_2021-08-24_21-45_epoch32</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, lr=0.01, decay epoch=[20, 30], centercrop test, crop 350x450, auto margin + scale during training</t>
+  </si>
+  <si>
+    <t>arccos margin weight_decay = 0.001, s=5, lr=0.01, decay epoch=[20, 30], centercrop test, crop 350x450, auto margin during training, dropout=0.2</t>
+  </si>
+  <si>
+    <t>efficientnet_b2_ArcMargin_2021-09-06_1-51_epoch99</t>
+  </si>
+  <si>
     <t xml:space="preserve">bad:
  - dropout
  - small batch
@@ -434,19 +454,149 @@
       'efficientnet-b7': (2.0, 3.1, 600, 0.5),
       'efficientnet-b8': (2.2, 3.6, 672, 0.5),
       'efficientnet-l2': (4.3, 5.3, 800, 0.5),
-  }	</t>
-  </si>
-  <si>
-    <t>densenet121_ArcMargin_2021-08-24_21-45_epoch32</t>
-  </si>
-  <si>
-    <t>arccos margin weight_decay = 0.001, lr=0.01, decay epoch=[20, 30], centercrop test, crop 350x450, auto margin + scale during training</t>
-  </si>
-  <si>
-    <t>arccos margin weight_decay = 0.001, s=5, lr=0.01, decay epoch=[20, 30], centercrop test, crop 350x450, auto margin during training, dropout=0.2</t>
-  </si>
-  <si>
-    <t>efficientnet_b2_ArcMargin_2021-09-06_1-51_epoch99</t>
+  }	
+</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>magnitude</t>
+  </si>
+  <si>
+    <t>op</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>sample pairing</t>
+  </si>
+  <si>
+    <t>rotate</t>
+  </si>
+  <si>
+    <t>[0, 0.4]</t>
+  </si>
+  <si>
+    <t>linearly add the image with another image (randomly selected from the same batch) with weight magnitude, without changing the label.</t>
+  </si>
+  <si>
+    <t>[-30, 30]</t>
+  </si>
+  <si>
+    <t>rotate image</t>
+  </si>
+  <si>
+    <t>gaussian noise</t>
+  </si>
+  <si>
+    <t>solarize add</t>
+  </si>
+  <si>
+    <t>[1, 110]</t>
+  </si>
+  <si>
+    <t>For each pixel in the image that is less than 128, add an additional amount to it decided by the magnitude</t>
+  </si>
+  <si>
+    <t>flip</t>
+  </si>
+  <si>
+    <t>cutout</t>
+  </si>
+  <si>
+    <t>[0, 60]</t>
+  </si>
+  <si>
+    <t>Set a random square patch of side-length magnitude pixels to gray.</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>shear X</t>
+  </si>
+  <si>
+    <t>[0.1, 1.9]</t>
+  </si>
+  <si>
+    <t>Adjust the color balance of the image, in a manner similar to the controls on a color TV set. A magnitude=0 gives a black &amp; white image, whereas magnitude=1 gives the original image.</t>
+  </si>
+  <si>
+    <t>[-0.3, 0.3]</t>
+  </si>
+  <si>
+    <t>Shear the image along the horizontal (vertical) axis with rate magnitude.</t>
+  </si>
+  <si>
+    <t>contrast</t>
+  </si>
+  <si>
+    <t>shear Y</t>
+  </si>
+  <si>
+    <t>Control the contrast of the image. A magnitude=0 gives a gray image, whereas magnitude=1 gives the original image</t>
+  </si>
+  <si>
+    <t>brightness</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>[0.6, 1.4]</t>
+  </si>
+  <si>
+    <t>Adjust the brightness of the image. A magnitude=0 gives a black image, whereas magnitude=1 gives the original image</t>
+  </si>
+  <si>
+    <t>Randomly scale the picture proportionally with rate magnitude.</t>
+  </si>
+  <si>
+    <t>sharpness</t>
+  </si>
+  <si>
+    <t>Adjust the sharpness of the image. A magnitude=0 gives a blurred image, whereas magnitude=1 gives the original image.</t>
+  </si>
+  <si>
+    <t>color shift</t>
+  </si>
+  <si>
+    <t>[-20, 20]</t>
+  </si>
+  <si>
+    <t>Add a random magnitude value to R, G, and B channels respectively</t>
+  </si>
+  <si>
+    <t>equalize YUV</t>
+  </si>
+  <si>
+    <t>[-03, 0.3]</t>
+  </si>
+  <si>
+    <t>Equalize the histogram of each YUV channel after transferring image into YUV color spaces.</t>
+  </si>
+  <si>
+    <t>posterize</t>
+  </si>
+  <si>
+    <t>[4, 8]</t>
+  </si>
+  <si>
+    <t>Reduce the number of bits for each pixel to magnitude bits</t>
+  </si>
+  <si>
+    <t>autocontrast</t>
+  </si>
+  <si>
+    <t>Maximize the image contrast, by making the darkest pixel black and lightest pixel white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equalize </t>
+  </si>
+  <si>
+    <t>Equalize the histogram of each RGB channel of image respectively</t>
   </si>
 </sst>
 </file>
@@ -523,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -562,12 +712,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1777,22 +1945,115 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>96385</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>257380</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2823216E-A52B-4EE2-9C64-50C3DAE386C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="123825"/>
+          <a:ext cx="8135485" cy="1467055"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>515681</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>210410</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D93C65-C078-4E8A-8DB4-29C64B688150}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9201150" y="1685925"/>
+          <a:ext cx="9535856" cy="6163535"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:I51" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{08419603-5237-4216-B2D3-9F0EA8121940}" name="Table1" displayName="Table1" ref="A1:I51" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:I51" xr:uid="{65955D23-65FA-4B98-9C71-606ABDF7F098}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I51">
     <sortCondition ref="E1:E51"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3E8B0DCA-57BB-461C-8A6E-9FA34A7B2BE6}" name="Architecture" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{87609125-158C-4CC5-AA8E-EEF050A67A7F}" name="Loss layer/function" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{E89C1E6C-8810-4E4B-B144-549BA40B4E4E}" name="Date" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{6E53C4CB-4A70-41F7-B3E6-AC55510650BC}" name="Voting" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{1ABD848E-ABED-4151-A1D7-F38492E6213F}" name="Batch size" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{9E6EDDE2-5951-49F3-BEC8-6D7190A570DA}" name="Epoch" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{5A7B834A-5526-436F-B0F7-AFB800C61477}" name="Model" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{80CDDCB1-6A70-4157-BB04-1D354CFF7BA2}" name="Score" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{3E8B0DCA-57BB-461C-8A6E-9FA34A7B2BE6}" name="Architecture" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{87609125-158C-4CC5-AA8E-EEF050A67A7F}" name="Loss layer/function" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{E89C1E6C-8810-4E4B-B144-549BA40B4E4E}" name="Date" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{6E53C4CB-4A70-41F7-B3E6-AC55510650BC}" name="Voting" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{1ABD848E-ABED-4151-A1D7-F38492E6213F}" name="Batch size" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{9E6EDDE2-5951-49F3-BEC8-6D7190A570DA}" name="Epoch" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A24A1274-F5B3-483F-B2C6-E8B35A9962E5}" name="Note" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1806,9 +2067,22 @@
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{BA1A0B66-9C88-496F-9F8A-5DCECE37CAF5}" name="model"/>
-    <tableColumn id="2" xr3:uid="{BB36172F-4C43-4AA6-A2BD-3C384E53BAB9}" name="no params" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{BB36172F-4C43-4AA6-A2BD-3C384E53BAB9}" name="no params" dataDxfId="5" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5F97048-196C-424E-8585-443AA87CBCDD}" name="Table3" displayName="Table3" ref="A1:D25" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:D25" xr:uid="{C5F97048-196C-424E-8585-443AA87CBCDD}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{571F61D0-C766-4A02-9884-10D35241F220}" name="policy" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{F2CDC32A-84E2-4FB6-845D-774361F93D06}" name="op" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DE27F8EF-2187-404A-9514-EDDEFDF4D84A}" name="magnitude" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{8B8E4431-BB5F-41C7-A541-D7E675EC928F}" name="description" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2077,7 +2351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -3159,7 +3433,7 @@
     </row>
     <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42" s="4">
         <v>0.75</v>
@@ -3180,7 +3454,7 @@
         <v>100</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3211,7 +3485,7 @@
     </row>
     <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" s="4">
         <v>0.751</v>
@@ -3232,7 +3506,7 @@
         <v>100</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3314,7 +3588,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3612,4 +3886,304 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB8F9A-DDEB-437D-94D1-566C22CC1365}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>4</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>5</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>6</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>8</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>10</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>11</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>12</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change dataloader back to normal (not using balanced batch sampler) remove redundant result files add untested low cost augment preprocess (center crop version) 16 crop version in-developing will refactor augmentation folder later update new result
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F6BF8-94D8-44CA-B2D0-44B72B20EDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CECB352-ABBA-476F-B580-A909A165E9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="164">
   <si>
     <t>Date</t>
   </si>
@@ -597,6 +600,15 @@
   </si>
   <si>
     <t>Equalize the histogram of each RGB channel of image respectively</t>
+  </si>
+  <si>
+    <t>ViT_ArcMargin_2022-02-14_18-58_epoch68</t>
+  </si>
+  <si>
+    <t>Vision Transformer</t>
+  </si>
+  <si>
+    <t>s=5, m=0.1 multiply by 0.1 at epoch 40, lr=0.01, decay epoch=[20, 30], centercrop test, crop 450x450, dropout=0.2, stock RandAugmentation, balanced batch sampler</t>
   </si>
 </sst>
 </file>
@@ -701,6 +713,9 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -711,9 +726,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -728,10 +740,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2074,11 +2086,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5F97048-196C-424E-8585-443AA87CBCDD}" name="Table3" displayName="Table3" ref="A1:D25" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C5F97048-196C-424E-8585-443AA87CBCDD}" name="Table3" displayName="Table3" ref="A1:D25" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D25" xr:uid="{C5F97048-196C-424E-8585-443AA87CBCDD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{571F61D0-C766-4A02-9884-10D35241F220}" name="policy" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{F2CDC32A-84E2-4FB6-845D-774361F93D06}" name="op" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{571F61D0-C766-4A02-9884-10D35241F220}" name="policy" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{F2CDC32A-84E2-4FB6-845D-774361F93D06}" name="op" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{DE27F8EF-2187-404A-9514-EDDEFDF4D84A}" name="magnitude" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{8B8E4431-BB5F-41C7-A541-D7E675EC928F}" name="description" dataDxfId="0"/>
   </tableColumns>
@@ -2351,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3509,8 +3521,31 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+    <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" s="7">
+        <v>44607</v>
+      </c>
+      <c r="G45" s="6">
+        <v>24</v>
+      </c>
+      <c r="H45" s="6">
+        <v>100</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
@@ -3557,11 +3592,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3583,11 +3618,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3892,14 +3927,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB8F9A-DDEB-437D-94D1-566C22CC1365}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="14.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="57.140625" style="8" customWidth="1"/>
   </cols>
@@ -3922,7 +3957,7 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>118</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -3933,7 +3968,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>119</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -3947,7 +3982,7 @@
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="10" t="s">
         <v>124</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -3955,7 +3990,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3963,7 +3998,7 @@
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -3974,7 +4009,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>129</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -3988,7 +4023,7 @@
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
         <v>132</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -3999,7 +4034,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="10" t="s">
         <v>133</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -4013,7 +4048,7 @@
       <c r="A10" s="4">
         <v>5</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="10" t="s">
         <v>138</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -4024,7 +4059,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="10" t="s">
         <v>139</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -4038,7 +4073,7 @@
       <c r="A12" s="4">
         <v>6</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="10" t="s">
         <v>141</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -4049,7 +4084,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>142</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -4063,7 +4098,7 @@
       <c r="A14" s="4">
         <v>7</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>146</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -4074,7 +4109,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="10" t="s">
         <v>119</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -4085,7 +4120,7 @@
       <c r="A16" s="4">
         <v>8</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>148</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -4096,7 +4131,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="10" t="s">
         <v>142</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -4107,7 +4142,7 @@
       <c r="A18" s="4">
         <v>9</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -4115,7 +4150,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>133</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -4126,7 +4161,7 @@
       <c r="A20" s="4">
         <v>10</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>154</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -4137,7 +4172,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="10" t="s">
         <v>139</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -4148,7 +4183,7 @@
       <c r="A22" s="4">
         <v>11</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
         <v>157</v>
       </c>
       <c r="D22" s="8" t="s">
@@ -4156,7 +4191,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4164,7 +4199,7 @@
       <c r="A24" s="4">
         <v>12</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="10" t="s">
         <v>159</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -4172,7 +4207,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="10" t="s">
         <v>129</v>
       </c>
       <c r="C25" s="4" t="s">

</xml_diff>

<commit_message>
fix sample sharing update new confusion matrix
</commit_message>
<xml_diff>
--- a/NOTES.xlsx
+++ b/NOTES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\thesisMs\SkinLesion\code\isic2018_Lesion-Diagnosis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CECB352-ABBA-476F-B580-A909A165E9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698B8374-1C06-4F42-A2E8-543E6DC79C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2363,7 +2363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>

</xml_diff>